<commit_message>
fix bugs to make writing data possible to-do: can not send file to user
</commit_message>
<xml_diff>
--- a/app/views/employees/review/TranKhanhThuan-review.xlsx
+++ b/app/views/employees/review/TranKhanhThuan-review.xlsx
@@ -2357,23 +2357,27 @@
       <c r="C3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
+      <c r="D3" s="3">
+        <v>4</v>
+      </c>
+      <c r="E3" s="3">
+        <v>4</v>
+      </c>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
       <c r="P3" s="14"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="14"/>
+      <c r="S3" s="14"/>
+      <c r="T3" s="14"/>
       <c r="U3" s="15" t="e">
         <f t="shared" ref="U3:U27" si="0">AVERAGE(D3:T3)</f>
         <v>#DIV/0!</v>
@@ -2393,23 +2397,27 @@
       <c r="C4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
+      <c r="D4" s="3">
+        <v>3</v>
+      </c>
+      <c r="E4" s="3">
+        <v>3</v>
+      </c>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
       <c r="P4" s="14"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="14"/>
       <c r="U4" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -2429,23 +2437,27 @@
       <c r="C5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
+      <c r="D5" s="3">
+        <v>3</v>
+      </c>
+      <c r="E5" s="3">
+        <v>3</v>
+      </c>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
       <c r="P5" s="14"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="14"/>
       <c r="U5" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -2468,23 +2480,27 @@
       <c r="C6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
+      <c r="D6" s="3">
+        <v>4</v>
+      </c>
+      <c r="E6" s="3">
+        <v>4</v>
+      </c>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
       <c r="P6" s="14"/>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="14"/>
+      <c r="T6" s="14"/>
       <c r="U6" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -2507,23 +2523,27 @@
       <c r="C7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
+      <c r="D7" s="3">
+        <v>3</v>
+      </c>
+      <c r="E7" s="3">
+        <v>3</v>
+      </c>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
       <c r="P7" s="14"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="14"/>
+      <c r="S7" s="14"/>
+      <c r="T7" s="14"/>
       <c r="U7" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -2543,23 +2563,27 @@
       <c r="C8" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
+      <c r="D8" s="3">
+        <v>4</v>
+      </c>
+      <c r="E8" s="3">
+        <v>4</v>
+      </c>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
       <c r="P8" s="14"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="14"/>
+      <c r="T8" s="14"/>
       <c r="U8" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -2582,23 +2606,27 @@
       <c r="C9" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
+      <c r="D9" s="3">
+        <v>3</v>
+      </c>
+      <c r="E9" s="3">
+        <v>3</v>
+      </c>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
       <c r="P9" s="14"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
-      <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="14"/>
       <c r="U9" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -2618,23 +2646,27 @@
       <c r="C10" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
+      <c r="D10" s="3">
+        <v>4</v>
+      </c>
+      <c r="E10" s="3">
+        <v>4</v>
+      </c>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
       <c r="P10" s="14"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
-      <c r="S10" s="3"/>
-      <c r="T10" s="3"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="14"/>
+      <c r="S10" s="14"/>
+      <c r="T10" s="14"/>
       <c r="U10" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -2654,23 +2686,27 @@
       <c r="C11" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
+      <c r="D11" s="3">
+        <v>4</v>
+      </c>
+      <c r="E11" s="3">
+        <v>4</v>
+      </c>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
       <c r="P11" s="14"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
-      <c r="S11" s="3"/>
-      <c r="T11" s="3"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14"/>
+      <c r="S11" s="14"/>
+      <c r="T11" s="14"/>
       <c r="U11" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -2693,23 +2729,27 @@
       <c r="C12" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
+      <c r="D12" s="3">
+        <v>4</v>
+      </c>
+      <c r="E12" s="3">
+        <v>4</v>
+      </c>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
       <c r="P12" s="14"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="3"/>
-      <c r="S12" s="3"/>
-      <c r="T12" s="3"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="14"/>
+      <c r="S12" s="14"/>
+      <c r="T12" s="14"/>
       <c r="U12" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -2729,23 +2769,27 @@
       <c r="C13" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
+      <c r="D13" s="3">
+        <v>3</v>
+      </c>
+      <c r="E13" s="3">
+        <v>3</v>
+      </c>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
       <c r="P13" s="14"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
-      <c r="S13" s="3"/>
-      <c r="T13" s="3"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="14"/>
+      <c r="S13" s="14"/>
+      <c r="T13" s="14"/>
       <c r="U13" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -2765,23 +2809,27 @@
       <c r="C14" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
+      <c r="D14" s="3">
+        <v>4</v>
+      </c>
+      <c r="E14" s="3">
+        <v>4</v>
+      </c>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
       <c r="P14" s="14"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="3"/>
-      <c r="S14" s="3"/>
-      <c r="T14" s="3"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="14"/>
       <c r="U14" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -2801,23 +2849,27 @@
       <c r="C15" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
+      <c r="D15" s="3">
+        <v>4</v>
+      </c>
+      <c r="E15" s="3">
+        <v>4</v>
+      </c>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
       <c r="P15" s="14"/>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="3"/>
-      <c r="S15" s="3"/>
-      <c r="T15" s="3"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="14"/>
       <c r="U15" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -2837,23 +2889,27 @@
       <c r="C16" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
+      <c r="D16" s="3">
+        <v>3</v>
+      </c>
+      <c r="E16" s="3">
+        <v>3</v>
+      </c>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
       <c r="P16" s="14"/>
-      <c r="Q16" s="3"/>
-      <c r="R16" s="3"/>
-      <c r="S16" s="3"/>
-      <c r="T16" s="3"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="14"/>
+      <c r="T16" s="14"/>
       <c r="U16" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -2876,23 +2932,27 @@
       <c r="C17" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
+      <c r="D17" s="3">
+        <v>4</v>
+      </c>
+      <c r="E17" s="3">
+        <v>4</v>
+      </c>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
       <c r="P17" s="14"/>
-      <c r="Q17" s="3"/>
-      <c r="R17" s="3"/>
-      <c r="S17" s="3"/>
-      <c r="T17" s="3"/>
+      <c r="Q17" s="14"/>
+      <c r="R17" s="14"/>
+      <c r="S17" s="14"/>
+      <c r="T17" s="14"/>
       <c r="U17" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -2912,23 +2972,27 @@
       <c r="C18" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
+      <c r="D18" s="3">
+        <v>4</v>
+      </c>
+      <c r="E18" s="3">
+        <v>4</v>
+      </c>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
       <c r="P18" s="14"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="3"/>
-      <c r="S18" s="3"/>
-      <c r="T18" s="3"/>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="14"/>
+      <c r="S18" s="14"/>
+      <c r="T18" s="14"/>
       <c r="U18" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -2948,23 +3012,27 @@
       <c r="C19" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
+      <c r="D19" s="3">
+        <v>3</v>
+      </c>
+      <c r="E19" s="3">
+        <v>3</v>
+      </c>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="14"/>
       <c r="P19" s="14"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
-      <c r="S19" s="3"/>
-      <c r="T19" s="3"/>
+      <c r="Q19" s="14"/>
+      <c r="R19" s="14"/>
+      <c r="S19" s="14"/>
+      <c r="T19" s="14"/>
       <c r="U19" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -2984,23 +3052,27 @@
       <c r="C20" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
+      <c r="D20" s="3">
+        <v>4</v>
+      </c>
+      <c r="E20" s="3">
+        <v>4</v>
+      </c>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
       <c r="P20" s="14"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="3"/>
-      <c r="T20" s="3"/>
+      <c r="Q20" s="14"/>
+      <c r="R20" s="14"/>
+      <c r="S20" s="14"/>
+      <c r="T20" s="14"/>
       <c r="U20" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3023,23 +3095,27 @@
       <c r="C21" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
+      <c r="D21" s="3">
+        <v>3</v>
+      </c>
+      <c r="E21" s="3">
+        <v>3</v>
+      </c>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="14"/>
       <c r="P21" s="14"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
-      <c r="S21" s="3"/>
-      <c r="T21" s="3"/>
+      <c r="Q21" s="14"/>
+      <c r="R21" s="14"/>
+      <c r="S21" s="14"/>
+      <c r="T21" s="14"/>
       <c r="U21" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3059,23 +3135,27 @@
       <c r="C22" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
+      <c r="D22" s="3">
+        <v>3</v>
+      </c>
+      <c r="E22" s="3">
+        <v>3</v>
+      </c>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="14"/>
+      <c r="O22" s="14"/>
       <c r="P22" s="14"/>
-      <c r="Q22" s="3"/>
-      <c r="R22" s="3"/>
-      <c r="S22" s="3"/>
-      <c r="T22" s="3"/>
+      <c r="Q22" s="14"/>
+      <c r="R22" s="14"/>
+      <c r="S22" s="14"/>
+      <c r="T22" s="14"/>
       <c r="U22" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3095,23 +3175,27 @@
       <c r="C23" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="3"/>
+      <c r="D23" s="3">
+        <v>4</v>
+      </c>
+      <c r="E23" s="3">
+        <v>4</v>
+      </c>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="18"/>
       <c r="P23" s="18"/>
-      <c r="Q23" s="3"/>
-      <c r="R23" s="3"/>
-      <c r="S23" s="3"/>
-      <c r="T23" s="3"/>
+      <c r="Q23" s="18"/>
+      <c r="R23" s="18"/>
+      <c r="S23" s="18"/>
+      <c r="T23" s="18"/>
       <c r="U23" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3131,22 +3215,12 @@
       <c r="C24" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="3"/>
-      <c r="Q24" s="3"/>
-      <c r="R24" s="3"/>
-      <c r="S24" s="3"/>
-      <c r="T24" s="3"/>
+      <c r="D24" s="3">
+        <v>3</v>
+      </c>
+      <c r="E24" s="3">
+        <v>3</v>
+      </c>
       <c r="U24" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3166,22 +3240,12 @@
       <c r="C25" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
-      <c r="O25" s="3"/>
-      <c r="Q25" s="3"/>
-      <c r="R25" s="3"/>
-      <c r="S25" s="3"/>
-      <c r="T25" s="3"/>
+      <c r="D25" s="3">
+        <v>4</v>
+      </c>
+      <c r="E25" s="3">
+        <v>4</v>
+      </c>
       <c r="U25" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3201,22 +3265,12 @@
       <c r="C26" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
-      <c r="O26" s="3"/>
-      <c r="Q26" s="3"/>
-      <c r="R26" s="3"/>
-      <c r="S26" s="3"/>
-      <c r="T26" s="3"/>
+      <c r="D26" s="3">
+        <v>3</v>
+      </c>
+      <c r="E26" s="3">
+        <v>3</v>
+      </c>
       <c r="U26" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3236,22 +3290,12 @@
       <c r="C27" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
-      <c r="O27" s="3"/>
-      <c r="Q27" s="3"/>
-      <c r="R27" s="3"/>
-      <c r="S27" s="3"/>
-      <c r="T27" s="3"/>
+      <c r="D27" s="3">
+        <v>4</v>
+      </c>
+      <c r="E27" s="3">
+        <v>4</v>
+      </c>
       <c r="U27" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3541,23 +3585,27 @@
         <v>47</v>
       </c>
       <c r="D3" s="41"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
+      <c r="E3" s="3">
+        <v>4</v>
+      </c>
+      <c r="F3" s="3">
+        <v>4</v>
+      </c>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
       <c r="Q3" s="14"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
+      <c r="R3" s="14"/>
+      <c r="S3" s="14"/>
+      <c r="T3" s="14"/>
+      <c r="U3" s="14"/>
       <c r="V3" s="15" t="e">
         <f>AVERAGE(E3:U3)</f>
         <v>#DIV/0!</v>
@@ -3581,23 +3629,27 @@
         <v>48</v>
       </c>
       <c r="D4" s="41"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
+      <c r="E4" s="3">
+        <v>3</v>
+      </c>
+      <c r="F4" s="3">
+        <v>3</v>
+      </c>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
       <c r="Q4" s="14"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="14"/>
+      <c r="U4" s="14"/>
       <c r="V4" s="15" t="e">
         <f t="shared" ref="V4:V27" si="0">AVERAGE(E4:U4)</f>
         <v>#DIV/0!</v>
@@ -3621,23 +3673,27 @@
         <v>49</v>
       </c>
       <c r="D5" s="41"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
+      <c r="E5" s="3">
+        <v>3</v>
+      </c>
+      <c r="F5" s="3">
+        <v>3</v>
+      </c>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
       <c r="Q5" s="14"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="14"/>
+      <c r="U5" s="14"/>
       <c r="V5" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3661,23 +3717,27 @@
         <v>50</v>
       </c>
       <c r="D6" s="43"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
+      <c r="E6" s="3">
+        <v>3</v>
+      </c>
+      <c r="F6" s="3">
+        <v>3</v>
+      </c>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
       <c r="Q6" s="14"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
-      <c r="U6" s="3"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="14"/>
+      <c r="T6" s="14"/>
+      <c r="U6" s="14"/>
       <c r="V6" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3701,23 +3761,27 @@
         <v>51</v>
       </c>
       <c r="D7" s="41"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
+      <c r="E7" s="3">
+        <v>3</v>
+      </c>
+      <c r="F7" s="3">
+        <v>3</v>
+      </c>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
       <c r="Q7" s="14"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
+      <c r="R7" s="14"/>
+      <c r="S7" s="14"/>
+      <c r="T7" s="14"/>
+      <c r="U7" s="14"/>
       <c r="V7" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3741,23 +3805,27 @@
         <v>53</v>
       </c>
       <c r="D8" s="41"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
+      <c r="E8" s="3">
+        <v>4</v>
+      </c>
+      <c r="F8" s="3">
+        <v>4</v>
+      </c>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
       <c r="Q8" s="14"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="U8" s="3"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="14"/>
+      <c r="T8" s="14"/>
+      <c r="U8" s="14"/>
       <c r="V8" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3781,23 +3849,27 @@
         <v>54</v>
       </c>
       <c r="D9" s="43"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
+      <c r="E9" s="3">
+        <v>4</v>
+      </c>
+      <c r="F9" s="3">
+        <v>4</v>
+      </c>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
       <c r="Q9" s="14"/>
-      <c r="R9" s="3"/>
-      <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
-      <c r="U9" s="3"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="14"/>
+      <c r="U9" s="14"/>
       <c r="V9" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3821,23 +3893,27 @@
         <v>55</v>
       </c>
       <c r="D10" s="41"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
+      <c r="E10" s="3">
+        <v>4</v>
+      </c>
+      <c r="F10" s="3">
+        <v>4</v>
+      </c>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
       <c r="Q10" s="14"/>
-      <c r="R10" s="3"/>
-      <c r="S10" s="3"/>
-      <c r="T10" s="3"/>
-      <c r="U10" s="3"/>
+      <c r="R10" s="14"/>
+      <c r="S10" s="14"/>
+      <c r="T10" s="14"/>
+      <c r="U10" s="14"/>
       <c r="V10" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3861,23 +3937,27 @@
         <v>56</v>
       </c>
       <c r="D11" s="41"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
+      <c r="E11" s="3">
+        <v>3</v>
+      </c>
+      <c r="F11" s="3">
+        <v>3</v>
+      </c>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
       <c r="Q11" s="14"/>
-      <c r="R11" s="3"/>
-      <c r="S11" s="3"/>
-      <c r="T11" s="3"/>
-      <c r="U11" s="3"/>
+      <c r="R11" s="14"/>
+      <c r="S11" s="14"/>
+      <c r="T11" s="14"/>
+      <c r="U11" s="14"/>
       <c r="V11" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3901,23 +3981,27 @@
         <v>57</v>
       </c>
       <c r="D12" s="41"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
+      <c r="E12" s="3">
+        <v>3</v>
+      </c>
+      <c r="F12" s="3">
+        <v>3</v>
+      </c>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
       <c r="Q12" s="14"/>
-      <c r="R12" s="3"/>
-      <c r="S12" s="3"/>
-      <c r="T12" s="3"/>
-      <c r="U12" s="3"/>
+      <c r="R12" s="14"/>
+      <c r="S12" s="14"/>
+      <c r="T12" s="14"/>
+      <c r="U12" s="14"/>
       <c r="V12" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3941,23 +4025,27 @@
         <v>59</v>
       </c>
       <c r="D13" s="41"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
+      <c r="E13" s="3">
+        <v>4</v>
+      </c>
+      <c r="F13" s="3">
+        <v>4</v>
+      </c>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="14"/>
       <c r="Q13" s="14"/>
-      <c r="R13" s="3"/>
-      <c r="S13" s="3"/>
-      <c r="T13" s="3"/>
-      <c r="U13" s="3"/>
+      <c r="R13" s="14"/>
+      <c r="S13" s="14"/>
+      <c r="T13" s="14"/>
+      <c r="U13" s="14"/>
       <c r="V13" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3981,23 +4069,27 @@
         <v>60</v>
       </c>
       <c r="D14" s="41"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
+      <c r="E14" s="3">
+        <v>3</v>
+      </c>
+      <c r="F14" s="3">
+        <v>3</v>
+      </c>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
       <c r="Q14" s="14"/>
-      <c r="R14" s="3"/>
-      <c r="S14" s="3"/>
-      <c r="T14" s="3"/>
-      <c r="U14" s="3"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="14"/>
+      <c r="U14" s="14"/>
       <c r="V14" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -4021,23 +4113,27 @@
         <v>61</v>
       </c>
       <c r="D15" s="41"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
+      <c r="E15" s="3">
+        <v>4</v>
+      </c>
+      <c r="F15" s="3">
+        <v>4</v>
+      </c>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
       <c r="Q15" s="14"/>
-      <c r="R15" s="3"/>
-      <c r="S15" s="3"/>
-      <c r="T15" s="3"/>
-      <c r="U15" s="3"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="14"/>
+      <c r="U15" s="14"/>
       <c r="V15" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -4061,23 +4157,27 @@
         <v>62</v>
       </c>
       <c r="D16" s="41"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
+      <c r="E16" s="3">
+        <v>4</v>
+      </c>
+      <c r="F16" s="3">
+        <v>4</v>
+      </c>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
       <c r="Q16" s="14"/>
-      <c r="R16" s="3"/>
-      <c r="S16" s="3"/>
-      <c r="T16" s="3"/>
-      <c r="U16" s="3"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="14"/>
+      <c r="T16" s="14"/>
+      <c r="U16" s="14"/>
       <c r="V16" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -4101,23 +4201,27 @@
         <v>63</v>
       </c>
       <c r="D17" s="41"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
+      <c r="E17" s="3">
+        <v>3</v>
+      </c>
+      <c r="F17" s="3">
+        <v>3</v>
+      </c>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
+      <c r="P17" s="14"/>
       <c r="Q17" s="14"/>
-      <c r="R17" s="3"/>
-      <c r="S17" s="3"/>
-      <c r="T17" s="3"/>
-      <c r="U17" s="3"/>
+      <c r="R17" s="14"/>
+      <c r="S17" s="14"/>
+      <c r="T17" s="14"/>
+      <c r="U17" s="14"/>
       <c r="V17" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -4141,23 +4245,27 @@
         <v>64</v>
       </c>
       <c r="D18" s="41"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
+      <c r="E18" s="3">
+        <v>4</v>
+      </c>
+      <c r="F18" s="3">
+        <v>4</v>
+      </c>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="14"/>
       <c r="Q18" s="14"/>
-      <c r="R18" s="3"/>
-      <c r="S18" s="3"/>
-      <c r="T18" s="3"/>
-      <c r="U18" s="3"/>
+      <c r="R18" s="14"/>
+      <c r="S18" s="14"/>
+      <c r="T18" s="14"/>
+      <c r="U18" s="14"/>
       <c r="V18" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -4181,23 +4289,27 @@
         <v>66</v>
       </c>
       <c r="D19" s="41"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
+      <c r="E19" s="3">
+        <v>3</v>
+      </c>
+      <c r="F19" s="3">
+        <v>3</v>
+      </c>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="14"/>
+      <c r="P19" s="14"/>
       <c r="Q19" s="14"/>
-      <c r="R19" s="3"/>
-      <c r="S19" s="3"/>
-      <c r="T19" s="3"/>
-      <c r="U19" s="3"/>
+      <c r="R19" s="14"/>
+      <c r="S19" s="14"/>
+      <c r="T19" s="14"/>
+      <c r="U19" s="14"/>
       <c r="V19" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -4221,23 +4333,27 @@
         <v>67</v>
       </c>
       <c r="D20" s="41"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
+      <c r="E20" s="3">
+        <v>3</v>
+      </c>
+      <c r="F20" s="3">
+        <v>3</v>
+      </c>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="14"/>
       <c r="Q20" s="14"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="3"/>
-      <c r="T20" s="3"/>
-      <c r="U20" s="3"/>
+      <c r="R20" s="14"/>
+      <c r="S20" s="14"/>
+      <c r="T20" s="14"/>
+      <c r="U20" s="14"/>
       <c r="V20" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -4261,23 +4377,27 @@
         <v>69</v>
       </c>
       <c r="D21" s="41"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
+      <c r="E21" s="3">
+        <v>3</v>
+      </c>
+      <c r="F21" s="3">
+        <v>3</v>
+      </c>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="14"/>
+      <c r="P21" s="14"/>
       <c r="Q21" s="14"/>
-      <c r="R21" s="3"/>
-      <c r="S21" s="3"/>
-      <c r="T21" s="3"/>
-      <c r="U21" s="3"/>
+      <c r="R21" s="14"/>
+      <c r="S21" s="14"/>
+      <c r="T21" s="14"/>
+      <c r="U21" s="14"/>
       <c r="V21" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -4301,23 +4421,27 @@
         <v>70</v>
       </c>
       <c r="D22" s="41"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
+      <c r="E22" s="3">
+        <v>4</v>
+      </c>
+      <c r="F22" s="3">
+        <v>4</v>
+      </c>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="14"/>
+      <c r="O22" s="14"/>
+      <c r="P22" s="14"/>
       <c r="Q22" s="14"/>
-      <c r="R22" s="3"/>
-      <c r="S22" s="3"/>
-      <c r="T22" s="3"/>
-      <c r="U22" s="3"/>
+      <c r="R22" s="14"/>
+      <c r="S22" s="14"/>
+      <c r="T22" s="14"/>
+      <c r="U22" s="14"/>
       <c r="V22" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -4341,23 +4465,27 @@
         <v>71</v>
       </c>
       <c r="D23" s="41"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
+      <c r="E23" s="3">
+        <v>4</v>
+      </c>
+      <c r="F23" s="3">
+        <v>4</v>
+      </c>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="18"/>
       <c r="Q23" s="18"/>
-      <c r="R23" s="3"/>
-      <c r="S23" s="3"/>
-      <c r="T23" s="3"/>
-      <c r="U23" s="3"/>
+      <c r="R23" s="18"/>
+      <c r="S23" s="18"/>
+      <c r="T23" s="18"/>
+      <c r="U23" s="18"/>
       <c r="V23" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -4381,22 +4509,12 @@
         <v>72</v>
       </c>
       <c r="D24" s="43"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
-      <c r="R24" s="3"/>
-      <c r="S24" s="3"/>
-      <c r="T24" s="3"/>
-      <c r="U24" s="3"/>
+      <c r="E24" s="3">
+        <v>3</v>
+      </c>
+      <c r="F24" s="3">
+        <v>3</v>
+      </c>
       <c r="V24" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -4420,22 +4538,12 @@
         <v>73</v>
       </c>
       <c r="D25" s="43"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
-      <c r="O25" s="3"/>
-      <c r="P25" s="3"/>
-      <c r="R25" s="3"/>
-      <c r="S25" s="3"/>
-      <c r="T25" s="3"/>
-      <c r="U25" s="3"/>
+      <c r="E25" s="3">
+        <v>4</v>
+      </c>
+      <c r="F25" s="3">
+        <v>4</v>
+      </c>
       <c r="V25" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -4459,22 +4567,12 @@
         <v>74</v>
       </c>
       <c r="D26" s="41"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
-      <c r="O26" s="3"/>
-      <c r="P26" s="3"/>
-      <c r="R26" s="3"/>
-      <c r="S26" s="3"/>
-      <c r="T26" s="3"/>
-      <c r="U26" s="3"/>
+      <c r="E26" s="3">
+        <v>4</v>
+      </c>
+      <c r="F26" s="3">
+        <v>4</v>
+      </c>
       <c r="V26" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -4498,22 +4596,12 @@
         <v>75</v>
       </c>
       <c r="D27" s="43"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
-      <c r="O27" s="3"/>
-      <c r="P27" s="3"/>
-      <c r="R27" s="3"/>
-      <c r="S27" s="3"/>
-      <c r="T27" s="3"/>
-      <c r="U27" s="3"/>
+      <c r="E27" s="3">
+        <v>4</v>
+      </c>
+      <c r="F27" s="3">
+        <v>4</v>
+      </c>
       <c r="V27" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -4833,22 +4921,12 @@
       <c r="D3" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
-      <c r="T3" s="14"/>
-      <c r="U3" s="14"/>
+      <c r="E3" s="14">
+        <v>4</v>
+      </c>
+      <c r="H3" s="14">
+        <v>4</v>
+      </c>
       <c r="V3" s="15" t="e">
         <f>AVERAGE(E3:U3)</f>
         <v>#DIV/0!</v>
@@ -4874,22 +4952,12 @@
       <c r="D4" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
-      <c r="R4" s="14"/>
-      <c r="S4" s="14"/>
-      <c r="T4" s="14"/>
-      <c r="U4" s="14"/>
+      <c r="E4" s="14">
+        <v>4</v>
+      </c>
+      <c r="H4" s="14">
+        <v>4</v>
+      </c>
       <c r="V4" s="15" t="e">
         <f t="shared" ref="V4:V22" si="0">AVERAGE(E4:U4)</f>
         <v>#DIV/0!</v>
@@ -4915,22 +4983,12 @@
       <c r="D5" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
-      <c r="R5" s="14"/>
-      <c r="S5" s="14"/>
-      <c r="T5" s="14"/>
-      <c r="U5" s="14"/>
+      <c r="E5" s="14">
+        <v>3</v>
+      </c>
+      <c r="H5" s="14">
+        <v>3</v>
+      </c>
       <c r="V5" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -4956,22 +5014,12 @@
       <c r="D6" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
-      <c r="R6" s="14"/>
-      <c r="S6" s="14"/>
-      <c r="T6" s="14"/>
-      <c r="U6" s="14"/>
+      <c r="E6" s="14">
+        <v>3</v>
+      </c>
+      <c r="H6" s="14">
+        <v>3</v>
+      </c>
       <c r="V6" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -4997,22 +5045,12 @@
       <c r="D7" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="R7" s="14"/>
-      <c r="S7" s="14"/>
-      <c r="T7" s="14"/>
-      <c r="U7" s="14"/>
+      <c r="E7" s="14">
+        <v>3</v>
+      </c>
+      <c r="H7" s="14">
+        <v>3</v>
+      </c>
       <c r="V7" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -5038,22 +5076,12 @@
       <c r="D8" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-      <c r="R8" s="14"/>
-      <c r="S8" s="14"/>
-      <c r="T8" s="14"/>
-      <c r="U8" s="14"/>
+      <c r="E8" s="14">
+        <v>4</v>
+      </c>
+      <c r="H8" s="14">
+        <v>4</v>
+      </c>
       <c r="V8" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -5079,22 +5107,12 @@
       <c r="D9" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
-      <c r="R9" s="14"/>
-      <c r="S9" s="14"/>
-      <c r="T9" s="14"/>
-      <c r="U9" s="14"/>
+      <c r="E9" s="14">
+        <v>4</v>
+      </c>
+      <c r="H9" s="14">
+        <v>4</v>
+      </c>
       <c r="V9" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -5120,22 +5138,12 @@
       <c r="D10" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
-      <c r="R10" s="14"/>
-      <c r="S10" s="14"/>
-      <c r="T10" s="14"/>
-      <c r="U10" s="14"/>
+      <c r="E10" s="14">
+        <v>4</v>
+      </c>
+      <c r="H10" s="14">
+        <v>4</v>
+      </c>
       <c r="V10" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -5161,22 +5169,12 @@
       <c r="D11" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
-      <c r="R11" s="14"/>
-      <c r="S11" s="14"/>
-      <c r="T11" s="14"/>
-      <c r="U11" s="14"/>
+      <c r="E11" s="14">
+        <v>3</v>
+      </c>
+      <c r="H11" s="14">
+        <v>3</v>
+      </c>
       <c r="V11" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -5202,22 +5200,12 @@
       <c r="D12" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="14"/>
-      <c r="R12" s="14"/>
-      <c r="S12" s="14"/>
-      <c r="T12" s="14"/>
-      <c r="U12" s="14"/>
+      <c r="E12" s="14">
+        <v>4</v>
+      </c>
+      <c r="H12" s="14">
+        <v>4</v>
+      </c>
       <c r="V12" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -5243,22 +5231,12 @@
       <c r="D13" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14"/>
-      <c r="R13" s="14"/>
-      <c r="S13" s="14"/>
-      <c r="T13" s="14"/>
-      <c r="U13" s="14"/>
+      <c r="E13" s="14">
+        <v>4</v>
+      </c>
+      <c r="H13" s="14">
+        <v>4</v>
+      </c>
       <c r="V13" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -5284,22 +5262,12 @@
       <c r="D14" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14"/>
-      <c r="R14" s="14"/>
-      <c r="S14" s="14"/>
-      <c r="T14" s="14"/>
-      <c r="U14" s="14"/>
+      <c r="E14" s="14">
+        <v>4</v>
+      </c>
+      <c r="H14" s="14">
+        <v>4</v>
+      </c>
       <c r="V14" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -5325,22 +5293,12 @@
       <c r="D15" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-      <c r="R15" s="14"/>
-      <c r="S15" s="14"/>
-      <c r="T15" s="14"/>
-      <c r="U15" s="14"/>
+      <c r="E15" s="14">
+        <v>4</v>
+      </c>
+      <c r="H15" s="14">
+        <v>4</v>
+      </c>
       <c r="V15" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -5366,22 +5324,12 @@
       <c r="D16" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="14"/>
-      <c r="R16" s="14"/>
-      <c r="S16" s="14"/>
-      <c r="T16" s="14"/>
-      <c r="U16" s="14"/>
+      <c r="E16" s="14">
+        <v>4</v>
+      </c>
+      <c r="H16" s="14">
+        <v>4</v>
+      </c>
       <c r="V16" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -5407,22 +5355,12 @@
       <c r="D17" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="14"/>
-      <c r="R17" s="14"/>
-      <c r="S17" s="14"/>
-      <c r="T17" s="14"/>
-      <c r="U17" s="14"/>
+      <c r="E17" s="14">
+        <v>4</v>
+      </c>
+      <c r="H17" s="14">
+        <v>4</v>
+      </c>
       <c r="V17" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -5448,22 +5386,12 @@
       <c r="D18" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="14"/>
-      <c r="O18" s="14"/>
-      <c r="P18" s="14"/>
-      <c r="R18" s="14"/>
-      <c r="S18" s="14"/>
-      <c r="T18" s="14"/>
-      <c r="U18" s="14"/>
+      <c r="E18" s="14">
+        <v>4</v>
+      </c>
+      <c r="H18" s="14">
+        <v>4</v>
+      </c>
       <c r="V18" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -5489,22 +5417,12 @@
       <c r="D19" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="14"/>
-      <c r="P19" s="14"/>
-      <c r="R19" s="14"/>
-      <c r="S19" s="14"/>
-      <c r="T19" s="14"/>
-      <c r="U19" s="14"/>
+      <c r="E19" s="14">
+        <v>3</v>
+      </c>
+      <c r="H19" s="14">
+        <v>3</v>
+      </c>
       <c r="V19" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -5530,22 +5448,12 @@
       <c r="D20" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
-      <c r="P20" s="14"/>
-      <c r="R20" s="14"/>
-      <c r="S20" s="14"/>
-      <c r="T20" s="14"/>
-      <c r="U20" s="14"/>
+      <c r="E20" s="14">
+        <v>4</v>
+      </c>
+      <c r="H20" s="14">
+        <v>4</v>
+      </c>
       <c r="V20" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -5571,22 +5479,12 @@
       <c r="D21" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
-      <c r="P21" s="14"/>
-      <c r="R21" s="14"/>
-      <c r="S21" s="14"/>
-      <c r="T21" s="14"/>
-      <c r="U21" s="14"/>
+      <c r="E21" s="14">
+        <v>4</v>
+      </c>
+      <c r="H21" s="14">
+        <v>4</v>
+      </c>
       <c r="V21" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -5612,22 +5510,12 @@
       <c r="D22" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="14"/>
-      <c r="O22" s="14"/>
-      <c r="P22" s="14"/>
-      <c r="R22" s="14"/>
-      <c r="S22" s="14"/>
-      <c r="T22" s="14"/>
-      <c r="U22" s="14"/>
+      <c r="E22" s="14">
+        <v>3</v>
+      </c>
+      <c r="H22" s="14">
+        <v>3</v>
+      </c>
       <c r="V22" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>

</xml_diff>

<commit_message>
fix error: file not sent to browser, analyzing data of sheet vai_tro add total formula for excel template
</commit_message>
<xml_diff>
--- a/app/views/employees/review/TranKhanhThuan-review.xlsx
+++ b/app/views/employees/review/TranKhanhThuan-review.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="考え方- tu_duy" sheetId="4" r:id="rId5"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="133" count="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="134" count="134">
   <si>
     <r>
       <t xml:space="preserve">考え方評価   </t>
@@ -1406,13 +1406,16 @@
   <si>
     <t xml:space="preserve">レビュー
 Review- NguyenQuangMinh</t>
+  </si>
+  <si>
+    <t>Tổng điểm review chéo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
-  <fonts count="29">
+  <fonts count="31">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1610,8 +1613,21 @@
       <family val="1"/>
       <sz val="12"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="128"/>
+      <family val="2"/>
+      <sz val="12"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <color rgb="FF000000"/>
+      <sz val="12"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1645,6 +1661,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.1499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.5999938962981048"/>
+        <bgColor rgb="FFE2EFD9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.5999938962981048"/>
+        <bgColor rgb="FFC6D9F0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.5999938962981048"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1751,7 +1785,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
@@ -1866,6 +1900,21 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="29" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="30" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="30" fillId="8" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2254,7 +2303,7 @@
   <dimension ref="A1:W37"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="D2" sqref="D2:T2"/>
@@ -2363,20 +2412,48 @@
       <c r="E3" s="3">
         <v>4</v>
       </c>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
+      <c r="F3" s="3">
+        <v>4</v>
+      </c>
+      <c r="G3" s="3">
+        <v>4</v>
+      </c>
+      <c r="H3" s="3">
+        <v>4</v>
+      </c>
+      <c r="I3" s="3">
+        <v>4</v>
+      </c>
+      <c r="J3" s="3">
+        <v>4</v>
+      </c>
+      <c r="K3" s="3">
+        <v>4</v>
+      </c>
+      <c r="L3" s="3">
+        <v>4</v>
+      </c>
+      <c r="M3" s="3">
+        <v>4</v>
+      </c>
+      <c r="N3" s="3">
+        <v>4</v>
+      </c>
+      <c r="O3" s="3">
+        <v>4</v>
+      </c>
+      <c r="P3" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>4</v>
+      </c>
+      <c r="R3" s="3">
+        <v>4</v>
+      </c>
+      <c r="S3" s="3">
+        <v>4</v>
+      </c>
       <c r="T3" s="14"/>
       <c r="U3" s="15" t="e">
         <f t="shared" ref="U3:U27" si="0">AVERAGE(D3:T3)</f>
@@ -2403,20 +2480,48 @@
       <c r="E4" s="3">
         <v>3</v>
       </c>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
-      <c r="S4" s="14"/>
+      <c r="F4" s="3">
+        <v>3</v>
+      </c>
+      <c r="G4" s="3">
+        <v>3</v>
+      </c>
+      <c r="H4" s="3">
+        <v>3</v>
+      </c>
+      <c r="I4" s="3">
+        <v>3</v>
+      </c>
+      <c r="J4" s="3">
+        <v>3</v>
+      </c>
+      <c r="K4" s="3">
+        <v>3</v>
+      </c>
+      <c r="L4" s="3">
+        <v>3</v>
+      </c>
+      <c r="M4" s="3">
+        <v>3</v>
+      </c>
+      <c r="N4" s="3">
+        <v>3</v>
+      </c>
+      <c r="O4" s="3">
+        <v>3</v>
+      </c>
+      <c r="P4" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>3</v>
+      </c>
+      <c r="R4" s="3">
+        <v>3</v>
+      </c>
+      <c r="S4" s="3">
+        <v>3</v>
+      </c>
       <c r="T4" s="14"/>
       <c r="U4" s="15" t="e">
         <f t="shared" si="0"/>
@@ -2443,20 +2548,48 @@
       <c r="E5" s="3">
         <v>3</v>
       </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="14"/>
-      <c r="S5" s="14"/>
+      <c r="F5" s="3">
+        <v>3</v>
+      </c>
+      <c r="G5" s="3">
+        <v>3</v>
+      </c>
+      <c r="H5" s="3">
+        <v>3</v>
+      </c>
+      <c r="I5" s="3">
+        <v>3</v>
+      </c>
+      <c r="J5" s="3">
+        <v>3</v>
+      </c>
+      <c r="K5" s="3">
+        <v>3</v>
+      </c>
+      <c r="L5" s="3">
+        <v>3</v>
+      </c>
+      <c r="M5" s="3">
+        <v>3</v>
+      </c>
+      <c r="N5" s="3">
+        <v>3</v>
+      </c>
+      <c r="O5" s="3">
+        <v>3</v>
+      </c>
+      <c r="P5" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>3</v>
+      </c>
+      <c r="R5" s="3">
+        <v>3</v>
+      </c>
+      <c r="S5" s="3">
+        <v>3</v>
+      </c>
       <c r="T5" s="14"/>
       <c r="U5" s="15" t="e">
         <f t="shared" si="0"/>
@@ -2486,20 +2619,48 @@
       <c r="E6" s="3">
         <v>4</v>
       </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="14"/>
-      <c r="S6" s="14"/>
+      <c r="F6" s="3">
+        <v>4</v>
+      </c>
+      <c r="G6" s="3">
+        <v>4</v>
+      </c>
+      <c r="H6" s="3">
+        <v>4</v>
+      </c>
+      <c r="I6" s="3">
+        <v>4</v>
+      </c>
+      <c r="J6" s="3">
+        <v>4</v>
+      </c>
+      <c r="K6" s="3">
+        <v>4</v>
+      </c>
+      <c r="L6" s="3">
+        <v>4</v>
+      </c>
+      <c r="M6" s="3">
+        <v>4</v>
+      </c>
+      <c r="N6" s="3">
+        <v>4</v>
+      </c>
+      <c r="O6" s="3">
+        <v>4</v>
+      </c>
+      <c r="P6" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>4</v>
+      </c>
+      <c r="R6" s="3">
+        <v>4</v>
+      </c>
+      <c r="S6" s="3">
+        <v>4</v>
+      </c>
       <c r="T6" s="14"/>
       <c r="U6" s="15" t="e">
         <f t="shared" si="0"/>
@@ -2529,20 +2690,48 @@
       <c r="E7" s="3">
         <v>3</v>
       </c>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
-      <c r="S7" s="14"/>
+      <c r="F7" s="3">
+        <v>3</v>
+      </c>
+      <c r="G7" s="3">
+        <v>3</v>
+      </c>
+      <c r="H7" s="3">
+        <v>3</v>
+      </c>
+      <c r="I7" s="3">
+        <v>3</v>
+      </c>
+      <c r="J7" s="3">
+        <v>3</v>
+      </c>
+      <c r="K7" s="3">
+        <v>3</v>
+      </c>
+      <c r="L7" s="3">
+        <v>3</v>
+      </c>
+      <c r="M7" s="3">
+        <v>3</v>
+      </c>
+      <c r="N7" s="3">
+        <v>3</v>
+      </c>
+      <c r="O7" s="3">
+        <v>3</v>
+      </c>
+      <c r="P7" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>3</v>
+      </c>
+      <c r="R7" s="3">
+        <v>3</v>
+      </c>
+      <c r="S7" s="3">
+        <v>3</v>
+      </c>
       <c r="T7" s="14"/>
       <c r="U7" s="15" t="e">
         <f t="shared" si="0"/>
@@ -2569,20 +2758,48 @@
       <c r="E8" s="3">
         <v>4</v>
       </c>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
-      <c r="S8" s="14"/>
+      <c r="F8" s="3">
+        <v>4</v>
+      </c>
+      <c r="G8" s="3">
+        <v>4</v>
+      </c>
+      <c r="H8" s="3">
+        <v>4</v>
+      </c>
+      <c r="I8" s="3">
+        <v>4</v>
+      </c>
+      <c r="J8" s="3">
+        <v>4</v>
+      </c>
+      <c r="K8" s="3">
+        <v>4</v>
+      </c>
+      <c r="L8" s="3">
+        <v>4</v>
+      </c>
+      <c r="M8" s="3">
+        <v>4</v>
+      </c>
+      <c r="N8" s="3">
+        <v>4</v>
+      </c>
+      <c r="O8" s="3">
+        <v>4</v>
+      </c>
+      <c r="P8" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>4</v>
+      </c>
+      <c r="R8" s="3">
+        <v>4</v>
+      </c>
+      <c r="S8" s="3">
+        <v>4</v>
+      </c>
       <c r="T8" s="14"/>
       <c r="U8" s="15" t="e">
         <f t="shared" si="0"/>
@@ -2612,20 +2829,48 @@
       <c r="E9" s="3">
         <v>3</v>
       </c>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
-      <c r="Q9" s="14"/>
-      <c r="R9" s="14"/>
-      <c r="S9" s="14"/>
+      <c r="F9" s="3">
+        <v>3</v>
+      </c>
+      <c r="G9" s="3">
+        <v>3</v>
+      </c>
+      <c r="H9" s="3">
+        <v>3</v>
+      </c>
+      <c r="I9" s="3">
+        <v>3</v>
+      </c>
+      <c r="J9" s="3">
+        <v>3</v>
+      </c>
+      <c r="K9" s="3">
+        <v>3</v>
+      </c>
+      <c r="L9" s="3">
+        <v>3</v>
+      </c>
+      <c r="M9" s="3">
+        <v>3</v>
+      </c>
+      <c r="N9" s="3">
+        <v>3</v>
+      </c>
+      <c r="O9" s="3">
+        <v>3</v>
+      </c>
+      <c r="P9" s="3">
+        <v>5</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>3</v>
+      </c>
+      <c r="R9" s="3">
+        <v>3</v>
+      </c>
+      <c r="S9" s="3">
+        <v>3</v>
+      </c>
       <c r="T9" s="14"/>
       <c r="U9" s="15" t="e">
         <f t="shared" si="0"/>
@@ -2652,20 +2897,48 @@
       <c r="E10" s="3">
         <v>4</v>
       </c>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="14"/>
-      <c r="R10" s="14"/>
-      <c r="S10" s="14"/>
+      <c r="F10" s="3">
+        <v>4</v>
+      </c>
+      <c r="G10" s="3">
+        <v>4</v>
+      </c>
+      <c r="H10" s="3">
+        <v>4</v>
+      </c>
+      <c r="I10" s="3">
+        <v>4</v>
+      </c>
+      <c r="J10" s="3">
+        <v>4</v>
+      </c>
+      <c r="K10" s="3">
+        <v>4</v>
+      </c>
+      <c r="L10" s="3">
+        <v>4</v>
+      </c>
+      <c r="M10" s="3">
+        <v>4</v>
+      </c>
+      <c r="N10" s="3">
+        <v>4</v>
+      </c>
+      <c r="O10" s="3">
+        <v>4</v>
+      </c>
+      <c r="P10" s="3">
+        <v>5</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>4</v>
+      </c>
+      <c r="R10" s="3">
+        <v>4</v>
+      </c>
+      <c r="S10" s="3">
+        <v>4</v>
+      </c>
       <c r="T10" s="14"/>
       <c r="U10" s="15" t="e">
         <f t="shared" si="0"/>
@@ -2692,20 +2965,48 @@
       <c r="E11" s="3">
         <v>4</v>
       </c>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
-      <c r="Q11" s="14"/>
-      <c r="R11" s="14"/>
-      <c r="S11" s="14"/>
+      <c r="F11" s="3">
+        <v>4</v>
+      </c>
+      <c r="G11" s="3">
+        <v>4</v>
+      </c>
+      <c r="H11" s="3">
+        <v>4</v>
+      </c>
+      <c r="I11" s="3">
+        <v>4</v>
+      </c>
+      <c r="J11" s="3">
+        <v>4</v>
+      </c>
+      <c r="K11" s="3">
+        <v>4</v>
+      </c>
+      <c r="L11" s="3">
+        <v>4</v>
+      </c>
+      <c r="M11" s="3">
+        <v>4</v>
+      </c>
+      <c r="N11" s="3">
+        <v>4</v>
+      </c>
+      <c r="O11" s="3">
+        <v>4</v>
+      </c>
+      <c r="P11" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>4</v>
+      </c>
+      <c r="R11" s="3">
+        <v>4</v>
+      </c>
+      <c r="S11" s="3">
+        <v>4</v>
+      </c>
       <c r="T11" s="14"/>
       <c r="U11" s="15" t="e">
         <f t="shared" si="0"/>
@@ -2735,20 +3036,48 @@
       <c r="E12" s="3">
         <v>4</v>
       </c>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="14"/>
-      <c r="R12" s="14"/>
-      <c r="S12" s="14"/>
+      <c r="F12" s="3">
+        <v>4</v>
+      </c>
+      <c r="G12" s="3">
+        <v>4</v>
+      </c>
+      <c r="H12" s="3">
+        <v>4</v>
+      </c>
+      <c r="I12" s="3">
+        <v>4</v>
+      </c>
+      <c r="J12" s="3">
+        <v>4</v>
+      </c>
+      <c r="K12" s="3">
+        <v>4</v>
+      </c>
+      <c r="L12" s="3">
+        <v>4</v>
+      </c>
+      <c r="M12" s="3">
+        <v>4</v>
+      </c>
+      <c r="N12" s="3">
+        <v>4</v>
+      </c>
+      <c r="O12" s="3">
+        <v>4</v>
+      </c>
+      <c r="P12" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>4</v>
+      </c>
+      <c r="R12" s="3">
+        <v>4</v>
+      </c>
+      <c r="S12" s="3">
+        <v>4</v>
+      </c>
       <c r="T12" s="14"/>
       <c r="U12" s="15" t="e">
         <f t="shared" si="0"/>
@@ -2775,20 +3104,48 @@
       <c r="E13" s="3">
         <v>3</v>
       </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="14"/>
-      <c r="R13" s="14"/>
-      <c r="S13" s="14"/>
+      <c r="F13" s="3">
+        <v>3</v>
+      </c>
+      <c r="G13" s="3">
+        <v>3</v>
+      </c>
+      <c r="H13" s="3">
+        <v>3</v>
+      </c>
+      <c r="I13" s="3">
+        <v>3</v>
+      </c>
+      <c r="J13" s="3">
+        <v>3</v>
+      </c>
+      <c r="K13" s="3">
+        <v>3</v>
+      </c>
+      <c r="L13" s="3">
+        <v>3</v>
+      </c>
+      <c r="M13" s="3">
+        <v>3</v>
+      </c>
+      <c r="N13" s="3">
+        <v>3</v>
+      </c>
+      <c r="O13" s="3">
+        <v>3</v>
+      </c>
+      <c r="P13" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>3</v>
+      </c>
+      <c r="R13" s="3">
+        <v>3</v>
+      </c>
+      <c r="S13" s="3">
+        <v>3</v>
+      </c>
       <c r="T13" s="14"/>
       <c r="U13" s="15" t="e">
         <f t="shared" si="0"/>
@@ -2815,20 +3172,48 @@
       <c r="E14" s="3">
         <v>4</v>
       </c>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="14"/>
-      <c r="S14" s="14"/>
+      <c r="F14" s="3">
+        <v>4</v>
+      </c>
+      <c r="G14" s="3">
+        <v>4</v>
+      </c>
+      <c r="H14" s="3">
+        <v>4</v>
+      </c>
+      <c r="I14" s="3">
+        <v>4</v>
+      </c>
+      <c r="J14" s="3">
+        <v>4</v>
+      </c>
+      <c r="K14" s="3">
+        <v>4</v>
+      </c>
+      <c r="L14" s="3">
+        <v>4</v>
+      </c>
+      <c r="M14" s="3">
+        <v>4</v>
+      </c>
+      <c r="N14" s="3">
+        <v>4</v>
+      </c>
+      <c r="O14" s="3">
+        <v>4</v>
+      </c>
+      <c r="P14" s="3">
+        <v>5</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>4</v>
+      </c>
+      <c r="R14" s="3">
+        <v>4</v>
+      </c>
+      <c r="S14" s="3">
+        <v>4</v>
+      </c>
       <c r="T14" s="14"/>
       <c r="U14" s="15" t="e">
         <f t="shared" si="0"/>
@@ -2855,20 +3240,48 @@
       <c r="E15" s="3">
         <v>4</v>
       </c>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="14"/>
-      <c r="S15" s="14"/>
+      <c r="F15" s="3">
+        <v>4</v>
+      </c>
+      <c r="G15" s="3">
+        <v>4</v>
+      </c>
+      <c r="H15" s="3">
+        <v>4</v>
+      </c>
+      <c r="I15" s="3">
+        <v>4</v>
+      </c>
+      <c r="J15" s="3">
+        <v>4</v>
+      </c>
+      <c r="K15" s="3">
+        <v>4</v>
+      </c>
+      <c r="L15" s="3">
+        <v>4</v>
+      </c>
+      <c r="M15" s="3">
+        <v>4</v>
+      </c>
+      <c r="N15" s="3">
+        <v>4</v>
+      </c>
+      <c r="O15" s="3">
+        <v>4</v>
+      </c>
+      <c r="P15" s="3">
+        <v>5</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>4</v>
+      </c>
+      <c r="R15" s="3">
+        <v>4</v>
+      </c>
+      <c r="S15" s="3">
+        <v>4</v>
+      </c>
       <c r="T15" s="14"/>
       <c r="U15" s="15" t="e">
         <f t="shared" si="0"/>
@@ -2895,20 +3308,48 @@
       <c r="E16" s="3">
         <v>3</v>
       </c>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="14"/>
-      <c r="S16" s="14"/>
+      <c r="F16" s="3">
+        <v>3</v>
+      </c>
+      <c r="G16" s="3">
+        <v>3</v>
+      </c>
+      <c r="H16" s="3">
+        <v>3</v>
+      </c>
+      <c r="I16" s="3">
+        <v>3</v>
+      </c>
+      <c r="J16" s="3">
+        <v>3</v>
+      </c>
+      <c r="K16" s="3">
+        <v>3</v>
+      </c>
+      <c r="L16" s="3">
+        <v>3</v>
+      </c>
+      <c r="M16" s="3">
+        <v>3</v>
+      </c>
+      <c r="N16" s="3">
+        <v>3</v>
+      </c>
+      <c r="O16" s="3">
+        <v>3</v>
+      </c>
+      <c r="P16" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>3</v>
+      </c>
+      <c r="R16" s="3">
+        <v>3</v>
+      </c>
+      <c r="S16" s="3">
+        <v>3</v>
+      </c>
       <c r="T16" s="14"/>
       <c r="U16" s="15" t="e">
         <f t="shared" si="0"/>
@@ -2938,20 +3379,48 @@
       <c r="E17" s="3">
         <v>4</v>
       </c>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="14"/>
-      <c r="Q17" s="14"/>
-      <c r="R17" s="14"/>
-      <c r="S17" s="14"/>
+      <c r="F17" s="3">
+        <v>4</v>
+      </c>
+      <c r="G17" s="3">
+        <v>4</v>
+      </c>
+      <c r="H17" s="3">
+        <v>4</v>
+      </c>
+      <c r="I17" s="3">
+        <v>4</v>
+      </c>
+      <c r="J17" s="3">
+        <v>4</v>
+      </c>
+      <c r="K17" s="3">
+        <v>4</v>
+      </c>
+      <c r="L17" s="3">
+        <v>4</v>
+      </c>
+      <c r="M17" s="3">
+        <v>4</v>
+      </c>
+      <c r="N17" s="3">
+        <v>4</v>
+      </c>
+      <c r="O17" s="3">
+        <v>4</v>
+      </c>
+      <c r="P17" s="3">
+        <v>5</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>4</v>
+      </c>
+      <c r="R17" s="3">
+        <v>4</v>
+      </c>
+      <c r="S17" s="3">
+        <v>4</v>
+      </c>
       <c r="T17" s="14"/>
       <c r="U17" s="15" t="e">
         <f t="shared" si="0"/>
@@ -2978,20 +3447,48 @@
       <c r="E18" s="3">
         <v>4</v>
       </c>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="14"/>
-      <c r="O18" s="14"/>
-      <c r="P18" s="14"/>
-      <c r="Q18" s="14"/>
-      <c r="R18" s="14"/>
-      <c r="S18" s="14"/>
+      <c r="F18" s="3">
+        <v>4</v>
+      </c>
+      <c r="G18" s="3">
+        <v>4</v>
+      </c>
+      <c r="H18" s="3">
+        <v>4</v>
+      </c>
+      <c r="I18" s="3">
+        <v>4</v>
+      </c>
+      <c r="J18" s="3">
+        <v>4</v>
+      </c>
+      <c r="K18" s="3">
+        <v>4</v>
+      </c>
+      <c r="L18" s="3">
+        <v>4</v>
+      </c>
+      <c r="M18" s="3">
+        <v>4</v>
+      </c>
+      <c r="N18" s="3">
+        <v>4</v>
+      </c>
+      <c r="O18" s="3">
+        <v>4</v>
+      </c>
+      <c r="P18" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>4</v>
+      </c>
+      <c r="R18" s="3">
+        <v>4</v>
+      </c>
+      <c r="S18" s="3">
+        <v>4</v>
+      </c>
       <c r="T18" s="14"/>
       <c r="U18" s="15" t="e">
         <f t="shared" si="0"/>
@@ -3018,20 +3515,48 @@
       <c r="E19" s="3">
         <v>3</v>
       </c>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="14"/>
-      <c r="P19" s="14"/>
-      <c r="Q19" s="14"/>
-      <c r="R19" s="14"/>
-      <c r="S19" s="14"/>
+      <c r="F19" s="3">
+        <v>3</v>
+      </c>
+      <c r="G19" s="3">
+        <v>3</v>
+      </c>
+      <c r="H19" s="3">
+        <v>3</v>
+      </c>
+      <c r="I19" s="3">
+        <v>3</v>
+      </c>
+      <c r="J19" s="3">
+        <v>3</v>
+      </c>
+      <c r="K19" s="3">
+        <v>3</v>
+      </c>
+      <c r="L19" s="3">
+        <v>3</v>
+      </c>
+      <c r="M19" s="3">
+        <v>3</v>
+      </c>
+      <c r="N19" s="3">
+        <v>3</v>
+      </c>
+      <c r="O19" s="3">
+        <v>3</v>
+      </c>
+      <c r="P19" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>3</v>
+      </c>
+      <c r="R19" s="3">
+        <v>3</v>
+      </c>
+      <c r="S19" s="3">
+        <v>3</v>
+      </c>
       <c r="T19" s="14"/>
       <c r="U19" s="15" t="e">
         <f t="shared" si="0"/>
@@ -3058,20 +3583,48 @@
       <c r="E20" s="3">
         <v>4</v>
       </c>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
-      <c r="P20" s="14"/>
-      <c r="Q20" s="14"/>
-      <c r="R20" s="14"/>
-      <c r="S20" s="14"/>
+      <c r="F20" s="3">
+        <v>4</v>
+      </c>
+      <c r="G20" s="3">
+        <v>4</v>
+      </c>
+      <c r="H20" s="3">
+        <v>4</v>
+      </c>
+      <c r="I20" s="3">
+        <v>4</v>
+      </c>
+      <c r="J20" s="3">
+        <v>4</v>
+      </c>
+      <c r="K20" s="3">
+        <v>4</v>
+      </c>
+      <c r="L20" s="3">
+        <v>4</v>
+      </c>
+      <c r="M20" s="3">
+        <v>4</v>
+      </c>
+      <c r="N20" s="3">
+        <v>4</v>
+      </c>
+      <c r="O20" s="3">
+        <v>4</v>
+      </c>
+      <c r="P20" s="3">
+        <v>5</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>4</v>
+      </c>
+      <c r="R20" s="3">
+        <v>4</v>
+      </c>
+      <c r="S20" s="3">
+        <v>4</v>
+      </c>
       <c r="T20" s="14"/>
       <c r="U20" s="15" t="e">
         <f t="shared" si="0"/>
@@ -3101,20 +3654,48 @@
       <c r="E21" s="3">
         <v>3</v>
       </c>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
-      <c r="P21" s="14"/>
-      <c r="Q21" s="14"/>
-      <c r="R21" s="14"/>
-      <c r="S21" s="14"/>
+      <c r="F21" s="3">
+        <v>3</v>
+      </c>
+      <c r="G21" s="3">
+        <v>3</v>
+      </c>
+      <c r="H21" s="3">
+        <v>3</v>
+      </c>
+      <c r="I21" s="3">
+        <v>3</v>
+      </c>
+      <c r="J21" s="3">
+        <v>3</v>
+      </c>
+      <c r="K21" s="3">
+        <v>3</v>
+      </c>
+      <c r="L21" s="3">
+        <v>3</v>
+      </c>
+      <c r="M21" s="3">
+        <v>3</v>
+      </c>
+      <c r="N21" s="3">
+        <v>3</v>
+      </c>
+      <c r="O21" s="3">
+        <v>3</v>
+      </c>
+      <c r="P21" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>3</v>
+      </c>
+      <c r="R21" s="3">
+        <v>3</v>
+      </c>
+      <c r="S21" s="3">
+        <v>3</v>
+      </c>
       <c r="T21" s="14"/>
       <c r="U21" s="15" t="e">
         <f t="shared" si="0"/>
@@ -3141,20 +3722,48 @@
       <c r="E22" s="3">
         <v>3</v>
       </c>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="14"/>
-      <c r="O22" s="14"/>
-      <c r="P22" s="14"/>
-      <c r="Q22" s="14"/>
-      <c r="R22" s="14"/>
-      <c r="S22" s="14"/>
+      <c r="F22" s="3">
+        <v>3</v>
+      </c>
+      <c r="G22" s="3">
+        <v>3</v>
+      </c>
+      <c r="H22" s="3">
+        <v>3</v>
+      </c>
+      <c r="I22" s="3">
+        <v>3</v>
+      </c>
+      <c r="J22" s="3">
+        <v>3</v>
+      </c>
+      <c r="K22" s="3">
+        <v>3</v>
+      </c>
+      <c r="L22" s="3">
+        <v>3</v>
+      </c>
+      <c r="M22" s="3">
+        <v>3</v>
+      </c>
+      <c r="N22" s="3">
+        <v>3</v>
+      </c>
+      <c r="O22" s="3">
+        <v>3</v>
+      </c>
+      <c r="P22" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>3</v>
+      </c>
+      <c r="R22" s="3">
+        <v>3</v>
+      </c>
+      <c r="S22" s="3">
+        <v>3</v>
+      </c>
       <c r="T22" s="14"/>
       <c r="U22" s="15" t="e">
         <f t="shared" si="0"/>
@@ -3181,20 +3790,48 @@
       <c r="E23" s="3">
         <v>4</v>
       </c>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
-      <c r="N23" s="18"/>
-      <c r="O23" s="18"/>
-      <c r="P23" s="18"/>
-      <c r="Q23" s="18"/>
-      <c r="R23" s="18"/>
-      <c r="S23" s="18"/>
+      <c r="F23" s="3">
+        <v>4</v>
+      </c>
+      <c r="G23" s="3">
+        <v>4</v>
+      </c>
+      <c r="H23" s="3">
+        <v>4</v>
+      </c>
+      <c r="I23" s="3">
+        <v>4</v>
+      </c>
+      <c r="J23" s="3">
+        <v>4</v>
+      </c>
+      <c r="K23" s="3">
+        <v>4</v>
+      </c>
+      <c r="L23" s="3">
+        <v>4</v>
+      </c>
+      <c r="M23" s="3">
+        <v>4</v>
+      </c>
+      <c r="N23" s="3">
+        <v>4</v>
+      </c>
+      <c r="O23" s="3">
+        <v>4</v>
+      </c>
+      <c r="P23" s="3">
+        <v>5</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>4</v>
+      </c>
+      <c r="R23" s="3">
+        <v>4</v>
+      </c>
+      <c r="S23" s="3">
+        <v>4</v>
+      </c>
       <c r="T23" s="18"/>
       <c r="U23" s="15" t="e">
         <f t="shared" si="0"/>
@@ -3221,6 +3858,48 @@
       <c r="E24" s="3">
         <v>3</v>
       </c>
+      <c r="F24" s="3">
+        <v>3</v>
+      </c>
+      <c r="G24" s="3">
+        <v>3</v>
+      </c>
+      <c r="H24" s="3">
+        <v>3</v>
+      </c>
+      <c r="I24" s="3">
+        <v>3</v>
+      </c>
+      <c r="J24" s="3">
+        <v>3</v>
+      </c>
+      <c r="K24" s="3">
+        <v>3</v>
+      </c>
+      <c r="L24" s="3">
+        <v>3</v>
+      </c>
+      <c r="M24" s="3">
+        <v>3</v>
+      </c>
+      <c r="N24" s="3">
+        <v>3</v>
+      </c>
+      <c r="O24" s="3">
+        <v>3</v>
+      </c>
+      <c r="P24" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>3</v>
+      </c>
+      <c r="R24" s="3">
+        <v>3</v>
+      </c>
+      <c r="S24" s="3">
+        <v>3</v>
+      </c>
       <c r="U24" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3246,6 +3925,48 @@
       <c r="E25" s="3">
         <v>4</v>
       </c>
+      <c r="F25" s="3">
+        <v>4</v>
+      </c>
+      <c r="G25" s="3">
+        <v>4</v>
+      </c>
+      <c r="H25" s="3">
+        <v>4</v>
+      </c>
+      <c r="I25" s="3">
+        <v>4</v>
+      </c>
+      <c r="J25" s="3">
+        <v>4</v>
+      </c>
+      <c r="K25" s="3">
+        <v>4</v>
+      </c>
+      <c r="L25" s="3">
+        <v>4</v>
+      </c>
+      <c r="M25" s="3">
+        <v>4</v>
+      </c>
+      <c r="N25" s="3">
+        <v>4</v>
+      </c>
+      <c r="O25" s="3">
+        <v>4</v>
+      </c>
+      <c r="P25" s="3">
+        <v>5</v>
+      </c>
+      <c r="Q25" s="3">
+        <v>4</v>
+      </c>
+      <c r="R25" s="3">
+        <v>4</v>
+      </c>
+      <c r="S25" s="3">
+        <v>4</v>
+      </c>
       <c r="U25" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3271,6 +3992,48 @@
       <c r="E26" s="3">
         <v>3</v>
       </c>
+      <c r="F26" s="3">
+        <v>3</v>
+      </c>
+      <c r="G26" s="3">
+        <v>3</v>
+      </c>
+      <c r="H26" s="3">
+        <v>3</v>
+      </c>
+      <c r="I26" s="3">
+        <v>3</v>
+      </c>
+      <c r="J26" s="3">
+        <v>3</v>
+      </c>
+      <c r="K26" s="3">
+        <v>3</v>
+      </c>
+      <c r="L26" s="3">
+        <v>3</v>
+      </c>
+      <c r="M26" s="3">
+        <v>3</v>
+      </c>
+      <c r="N26" s="3">
+        <v>3</v>
+      </c>
+      <c r="O26" s="3">
+        <v>3</v>
+      </c>
+      <c r="P26" s="3">
+        <v>5</v>
+      </c>
+      <c r="Q26" s="3">
+        <v>3</v>
+      </c>
+      <c r="R26" s="3">
+        <v>3</v>
+      </c>
+      <c r="S26" s="3">
+        <v>3</v>
+      </c>
       <c r="U26" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3296,6 +4059,48 @@
       <c r="E27" s="3">
         <v>4</v>
       </c>
+      <c r="F27" s="3">
+        <v>4</v>
+      </c>
+      <c r="G27" s="3">
+        <v>4</v>
+      </c>
+      <c r="H27" s="3">
+        <v>4</v>
+      </c>
+      <c r="I27" s="3">
+        <v>4</v>
+      </c>
+      <c r="J27" s="3">
+        <v>4</v>
+      </c>
+      <c r="K27" s="3">
+        <v>4</v>
+      </c>
+      <c r="L27" s="3">
+        <v>4</v>
+      </c>
+      <c r="M27" s="3">
+        <v>4</v>
+      </c>
+      <c r="N27" s="3">
+        <v>4</v>
+      </c>
+      <c r="O27" s="3">
+        <v>4</v>
+      </c>
+      <c r="P27" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q27" s="3">
+        <v>4</v>
+      </c>
+      <c r="R27" s="3">
+        <v>4</v>
+      </c>
+      <c r="S27" s="3">
+        <v>4</v>
+      </c>
       <c r="U27" s="15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3309,10 +4114,10 @@
       </c>
     </row>
     <row r="28" spans="2:23" customFormat="false">
-      <c r="B28" s="39" t="s">
+      <c r="B28" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="39"/>
+      <c r="C28" s="44"/>
       <c r="D28" s="3">
         <f>SUM(D3:D27)</f>
         <v>0</v>
@@ -3474,7 +4279,7 @@
   </sheetPr>
   <dimension ref="A1:X36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -3581,30 +4386,58 @@
       <c r="B3" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="41"/>
+      <c r="D3" s="46"/>
       <c r="E3" s="3">
         <v>4</v>
       </c>
       <c r="F3" s="3">
         <v>4</v>
       </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
-      <c r="T3" s="14"/>
+      <c r="G3" s="3">
+        <v>4</v>
+      </c>
+      <c r="H3" s="3">
+        <v>4</v>
+      </c>
+      <c r="I3" s="3">
+        <v>4</v>
+      </c>
+      <c r="J3" s="3">
+        <v>4</v>
+      </c>
+      <c r="K3" s="3">
+        <v>4</v>
+      </c>
+      <c r="L3" s="3">
+        <v>4</v>
+      </c>
+      <c r="M3" s="3">
+        <v>4</v>
+      </c>
+      <c r="N3" s="3">
+        <v>4</v>
+      </c>
+      <c r="O3" s="3">
+        <v>4</v>
+      </c>
+      <c r="P3" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>4</v>
+      </c>
+      <c r="R3" s="3">
+        <v>4</v>
+      </c>
+      <c r="S3" s="3">
+        <v>4</v>
+      </c>
+      <c r="T3" s="3">
+        <v>4</v>
+      </c>
       <c r="U3" s="14"/>
       <c r="V3" s="15" t="e">
         <f>AVERAGE(E3:U3)</f>
@@ -3625,30 +4458,58 @@
       <c r="B4" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="41"/>
+      <c r="D4" s="46"/>
       <c r="E4" s="3">
         <v>3</v>
       </c>
       <c r="F4" s="3">
         <v>3</v>
       </c>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
-      <c r="S4" s="14"/>
-      <c r="T4" s="14"/>
+      <c r="G4" s="3">
+        <v>3</v>
+      </c>
+      <c r="H4" s="3">
+        <v>3</v>
+      </c>
+      <c r="I4" s="3">
+        <v>3</v>
+      </c>
+      <c r="J4" s="3">
+        <v>3</v>
+      </c>
+      <c r="K4" s="3">
+        <v>3</v>
+      </c>
+      <c r="L4" s="3">
+        <v>3</v>
+      </c>
+      <c r="M4" s="3">
+        <v>3</v>
+      </c>
+      <c r="N4" s="3">
+        <v>3</v>
+      </c>
+      <c r="O4" s="3">
+        <v>3</v>
+      </c>
+      <c r="P4" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>3</v>
+      </c>
+      <c r="R4" s="3">
+        <v>3</v>
+      </c>
+      <c r="S4" s="3">
+        <v>3</v>
+      </c>
+      <c r="T4" s="3">
+        <v>3</v>
+      </c>
       <c r="U4" s="14"/>
       <c r="V4" s="15" t="e">
         <f t="shared" ref="V4:V27" si="0">AVERAGE(E4:U4)</f>
@@ -3669,30 +4530,58 @@
       <c r="B5" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="41"/>
+      <c r="D5" s="46"/>
       <c r="E5" s="3">
         <v>3</v>
       </c>
       <c r="F5" s="3">
         <v>3</v>
       </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="14"/>
-      <c r="S5" s="14"/>
-      <c r="T5" s="14"/>
+      <c r="G5" s="3">
+        <v>3</v>
+      </c>
+      <c r="H5" s="3">
+        <v>3</v>
+      </c>
+      <c r="I5" s="3">
+        <v>3</v>
+      </c>
+      <c r="J5" s="3">
+        <v>3</v>
+      </c>
+      <c r="K5" s="3">
+        <v>3</v>
+      </c>
+      <c r="L5" s="3">
+        <v>3</v>
+      </c>
+      <c r="M5" s="3">
+        <v>3</v>
+      </c>
+      <c r="N5" s="3">
+        <v>3</v>
+      </c>
+      <c r="O5" s="3">
+        <v>3</v>
+      </c>
+      <c r="P5" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>3</v>
+      </c>
+      <c r="R5" s="3">
+        <v>3</v>
+      </c>
+      <c r="S5" s="3">
+        <v>3</v>
+      </c>
+      <c r="T5" s="3">
+        <v>3</v>
+      </c>
       <c r="U5" s="14"/>
       <c r="V5" s="15" t="e">
         <f t="shared" si="0"/>
@@ -3713,30 +4602,58 @@
       <c r="B6" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="43"/>
+      <c r="D6" s="48"/>
       <c r="E6" s="3">
         <v>3</v>
       </c>
       <c r="F6" s="3">
         <v>3</v>
       </c>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="14"/>
-      <c r="S6" s="14"/>
-      <c r="T6" s="14"/>
+      <c r="G6" s="3">
+        <v>3</v>
+      </c>
+      <c r="H6" s="3">
+        <v>3</v>
+      </c>
+      <c r="I6" s="3">
+        <v>3</v>
+      </c>
+      <c r="J6" s="3">
+        <v>3</v>
+      </c>
+      <c r="K6" s="3">
+        <v>3</v>
+      </c>
+      <c r="L6" s="3">
+        <v>3</v>
+      </c>
+      <c r="M6" s="3">
+        <v>3</v>
+      </c>
+      <c r="N6" s="3">
+        <v>3</v>
+      </c>
+      <c r="O6" s="3">
+        <v>3</v>
+      </c>
+      <c r="P6" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>3</v>
+      </c>
+      <c r="R6" s="3">
+        <v>3</v>
+      </c>
+      <c r="S6" s="3">
+        <v>3</v>
+      </c>
+      <c r="T6" s="3">
+        <v>3</v>
+      </c>
       <c r="U6" s="14"/>
       <c r="V6" s="15" t="e">
         <f t="shared" si="0"/>
@@ -3757,30 +4674,58 @@
       <c r="B7" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="C7" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="41"/>
+      <c r="D7" s="46"/>
       <c r="E7" s="3">
         <v>3</v>
       </c>
       <c r="F7" s="3">
         <v>3</v>
       </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
-      <c r="S7" s="14"/>
-      <c r="T7" s="14"/>
+      <c r="G7" s="3">
+        <v>3</v>
+      </c>
+      <c r="H7" s="3">
+        <v>3</v>
+      </c>
+      <c r="I7" s="3">
+        <v>3</v>
+      </c>
+      <c r="J7" s="3">
+        <v>3</v>
+      </c>
+      <c r="K7" s="3">
+        <v>3</v>
+      </c>
+      <c r="L7" s="3">
+        <v>3</v>
+      </c>
+      <c r="M7" s="3">
+        <v>3</v>
+      </c>
+      <c r="N7" s="3">
+        <v>3</v>
+      </c>
+      <c r="O7" s="3">
+        <v>3</v>
+      </c>
+      <c r="P7" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>3</v>
+      </c>
+      <c r="R7" s="3">
+        <v>3</v>
+      </c>
+      <c r="S7" s="3">
+        <v>3</v>
+      </c>
+      <c r="T7" s="3">
+        <v>3</v>
+      </c>
       <c r="U7" s="14"/>
       <c r="V7" s="15" t="e">
         <f t="shared" si="0"/>
@@ -3801,30 +4746,58 @@
       <c r="B8" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="41"/>
+      <c r="D8" s="46"/>
       <c r="E8" s="3">
         <v>4</v>
       </c>
       <c r="F8" s="3">
         <v>4</v>
       </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
-      <c r="S8" s="14"/>
-      <c r="T8" s="14"/>
+      <c r="G8" s="3">
+        <v>4</v>
+      </c>
+      <c r="H8" s="3">
+        <v>4</v>
+      </c>
+      <c r="I8" s="3">
+        <v>4</v>
+      </c>
+      <c r="J8" s="3">
+        <v>4</v>
+      </c>
+      <c r="K8" s="3">
+        <v>4</v>
+      </c>
+      <c r="L8" s="3">
+        <v>4</v>
+      </c>
+      <c r="M8" s="3">
+        <v>4</v>
+      </c>
+      <c r="N8" s="3">
+        <v>4</v>
+      </c>
+      <c r="O8" s="3">
+        <v>4</v>
+      </c>
+      <c r="P8" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>4</v>
+      </c>
+      <c r="R8" s="3">
+        <v>4</v>
+      </c>
+      <c r="S8" s="3">
+        <v>4</v>
+      </c>
+      <c r="T8" s="3">
+        <v>4</v>
+      </c>
       <c r="U8" s="14"/>
       <c r="V8" s="15" t="e">
         <f t="shared" si="0"/>
@@ -3845,30 +4818,58 @@
       <c r="B9" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="43"/>
+      <c r="D9" s="48"/>
       <c r="E9" s="3">
         <v>4</v>
       </c>
       <c r="F9" s="3">
         <v>4</v>
       </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
-      <c r="Q9" s="14"/>
-      <c r="R9" s="14"/>
-      <c r="S9" s="14"/>
-      <c r="T9" s="14"/>
+      <c r="G9" s="3">
+        <v>4</v>
+      </c>
+      <c r="H9" s="3">
+        <v>4</v>
+      </c>
+      <c r="I9" s="3">
+        <v>4</v>
+      </c>
+      <c r="J9" s="3">
+        <v>4</v>
+      </c>
+      <c r="K9" s="3">
+        <v>4</v>
+      </c>
+      <c r="L9" s="3">
+        <v>4</v>
+      </c>
+      <c r="M9" s="3">
+        <v>4</v>
+      </c>
+      <c r="N9" s="3">
+        <v>4</v>
+      </c>
+      <c r="O9" s="3">
+        <v>4</v>
+      </c>
+      <c r="P9" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>4</v>
+      </c>
+      <c r="R9" s="3">
+        <v>4</v>
+      </c>
+      <c r="S9" s="3">
+        <v>4</v>
+      </c>
+      <c r="T9" s="3">
+        <v>4</v>
+      </c>
       <c r="U9" s="14"/>
       <c r="V9" s="15" t="e">
         <f t="shared" si="0"/>
@@ -3889,30 +4890,58 @@
       <c r="B10" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="40" t="s">
+      <c r="C10" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="41"/>
+      <c r="D10" s="46"/>
       <c r="E10" s="3">
         <v>4</v>
       </c>
       <c r="F10" s="3">
         <v>4</v>
       </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="14"/>
-      <c r="R10" s="14"/>
-      <c r="S10" s="14"/>
-      <c r="T10" s="14"/>
+      <c r="G10" s="3">
+        <v>4</v>
+      </c>
+      <c r="H10" s="3">
+        <v>4</v>
+      </c>
+      <c r="I10" s="3">
+        <v>4</v>
+      </c>
+      <c r="J10" s="3">
+        <v>4</v>
+      </c>
+      <c r="K10" s="3">
+        <v>4</v>
+      </c>
+      <c r="L10" s="3">
+        <v>4</v>
+      </c>
+      <c r="M10" s="3">
+        <v>4</v>
+      </c>
+      <c r="N10" s="3">
+        <v>4</v>
+      </c>
+      <c r="O10" s="3">
+        <v>4</v>
+      </c>
+      <c r="P10" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>4</v>
+      </c>
+      <c r="R10" s="3">
+        <v>4</v>
+      </c>
+      <c r="S10" s="3">
+        <v>4</v>
+      </c>
+      <c r="T10" s="3">
+        <v>4</v>
+      </c>
       <c r="U10" s="14"/>
       <c r="V10" s="15" t="e">
         <f t="shared" si="0"/>
@@ -3933,30 +4962,58 @@
       <c r="B11" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="40" t="s">
+      <c r="C11" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="41"/>
+      <c r="D11" s="46"/>
       <c r="E11" s="3">
         <v>3</v>
       </c>
       <c r="F11" s="3">
         <v>3</v>
       </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
-      <c r="Q11" s="14"/>
-      <c r="R11" s="14"/>
-      <c r="S11" s="14"/>
-      <c r="T11" s="14"/>
+      <c r="G11" s="3">
+        <v>3</v>
+      </c>
+      <c r="H11" s="3">
+        <v>3</v>
+      </c>
+      <c r="I11" s="3">
+        <v>3</v>
+      </c>
+      <c r="J11" s="3">
+        <v>3</v>
+      </c>
+      <c r="K11" s="3">
+        <v>3</v>
+      </c>
+      <c r="L11" s="3">
+        <v>3</v>
+      </c>
+      <c r="M11" s="3">
+        <v>3</v>
+      </c>
+      <c r="N11" s="3">
+        <v>3</v>
+      </c>
+      <c r="O11" s="3">
+        <v>3</v>
+      </c>
+      <c r="P11" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>3</v>
+      </c>
+      <c r="R11" s="3">
+        <v>3</v>
+      </c>
+      <c r="S11" s="3">
+        <v>3</v>
+      </c>
+      <c r="T11" s="3">
+        <v>3</v>
+      </c>
       <c r="U11" s="14"/>
       <c r="V11" s="15" t="e">
         <f t="shared" si="0"/>
@@ -3977,30 +5034,58 @@
       <c r="B12" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="D12" s="41"/>
+      <c r="D12" s="46"/>
       <c r="E12" s="3">
         <v>3</v>
       </c>
       <c r="F12" s="3">
         <v>3</v>
       </c>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="14"/>
-      <c r="R12" s="14"/>
-      <c r="S12" s="14"/>
-      <c r="T12" s="14"/>
+      <c r="G12" s="3">
+        <v>3</v>
+      </c>
+      <c r="H12" s="3">
+        <v>3</v>
+      </c>
+      <c r="I12" s="3">
+        <v>3</v>
+      </c>
+      <c r="J12" s="3">
+        <v>3</v>
+      </c>
+      <c r="K12" s="3">
+        <v>3</v>
+      </c>
+      <c r="L12" s="3">
+        <v>3</v>
+      </c>
+      <c r="M12" s="3">
+        <v>3</v>
+      </c>
+      <c r="N12" s="3">
+        <v>3</v>
+      </c>
+      <c r="O12" s="3">
+        <v>3</v>
+      </c>
+      <c r="P12" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>3</v>
+      </c>
+      <c r="R12" s="3">
+        <v>3</v>
+      </c>
+      <c r="S12" s="3">
+        <v>3</v>
+      </c>
+      <c r="T12" s="3">
+        <v>3</v>
+      </c>
       <c r="U12" s="14"/>
       <c r="V12" s="15" t="e">
         <f t="shared" si="0"/>
@@ -4021,30 +5106,58 @@
       <c r="B13" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="40" t="s">
+      <c r="C13" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="41"/>
+      <c r="D13" s="46"/>
       <c r="E13" s="3">
         <v>4</v>
       </c>
       <c r="F13" s="3">
         <v>4</v>
       </c>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="14"/>
-      <c r="R13" s="14"/>
-      <c r="S13" s="14"/>
-      <c r="T13" s="14"/>
+      <c r="G13" s="3">
+        <v>4</v>
+      </c>
+      <c r="H13" s="3">
+        <v>4</v>
+      </c>
+      <c r="I13" s="3">
+        <v>4</v>
+      </c>
+      <c r="J13" s="3">
+        <v>4</v>
+      </c>
+      <c r="K13" s="3">
+        <v>4</v>
+      </c>
+      <c r="L13" s="3">
+        <v>4</v>
+      </c>
+      <c r="M13" s="3">
+        <v>4</v>
+      </c>
+      <c r="N13" s="3">
+        <v>4</v>
+      </c>
+      <c r="O13" s="3">
+        <v>4</v>
+      </c>
+      <c r="P13" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>4</v>
+      </c>
+      <c r="R13" s="3">
+        <v>4</v>
+      </c>
+      <c r="S13" s="3">
+        <v>4</v>
+      </c>
+      <c r="T13" s="3">
+        <v>4</v>
+      </c>
       <c r="U13" s="14"/>
       <c r="V13" s="15" t="e">
         <f t="shared" si="0"/>
@@ -4065,30 +5178,58 @@
       <c r="B14" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="40" t="s">
+      <c r="C14" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="41"/>
+      <c r="D14" s="46"/>
       <c r="E14" s="3">
         <v>3</v>
       </c>
       <c r="F14" s="3">
         <v>3</v>
       </c>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="14"/>
-      <c r="S14" s="14"/>
-      <c r="T14" s="14"/>
+      <c r="G14" s="3">
+        <v>3</v>
+      </c>
+      <c r="H14" s="3">
+        <v>3</v>
+      </c>
+      <c r="I14" s="3">
+        <v>3</v>
+      </c>
+      <c r="J14" s="3">
+        <v>3</v>
+      </c>
+      <c r="K14" s="3">
+        <v>3</v>
+      </c>
+      <c r="L14" s="3">
+        <v>3</v>
+      </c>
+      <c r="M14" s="3">
+        <v>3</v>
+      </c>
+      <c r="N14" s="3">
+        <v>3</v>
+      </c>
+      <c r="O14" s="3">
+        <v>3</v>
+      </c>
+      <c r="P14" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>3</v>
+      </c>
+      <c r="R14" s="3">
+        <v>3</v>
+      </c>
+      <c r="S14" s="3">
+        <v>3</v>
+      </c>
+      <c r="T14" s="3">
+        <v>3</v>
+      </c>
       <c r="U14" s="14"/>
       <c r="V14" s="15" t="e">
         <f t="shared" si="0"/>
@@ -4109,30 +5250,58 @@
       <c r="B15" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="40" t="s">
+      <c r="C15" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="D15" s="41"/>
+      <c r="D15" s="46"/>
       <c r="E15" s="3">
         <v>4</v>
       </c>
       <c r="F15" s="3">
         <v>4</v>
       </c>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="14"/>
-      <c r="S15" s="14"/>
-      <c r="T15" s="14"/>
+      <c r="G15" s="3">
+        <v>4</v>
+      </c>
+      <c r="H15" s="3">
+        <v>4</v>
+      </c>
+      <c r="I15" s="3">
+        <v>4</v>
+      </c>
+      <c r="J15" s="3">
+        <v>4</v>
+      </c>
+      <c r="K15" s="3">
+        <v>4</v>
+      </c>
+      <c r="L15" s="3">
+        <v>4</v>
+      </c>
+      <c r="M15" s="3">
+        <v>4</v>
+      </c>
+      <c r="N15" s="3">
+        <v>4</v>
+      </c>
+      <c r="O15" s="3">
+        <v>4</v>
+      </c>
+      <c r="P15" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>4</v>
+      </c>
+      <c r="R15" s="3">
+        <v>4</v>
+      </c>
+      <c r="S15" s="3">
+        <v>4</v>
+      </c>
+      <c r="T15" s="3">
+        <v>4</v>
+      </c>
       <c r="U15" s="14"/>
       <c r="V15" s="15" t="e">
         <f t="shared" si="0"/>
@@ -4153,30 +5322,58 @@
       <c r="B16" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="40" t="s">
+      <c r="C16" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="D16" s="41"/>
+      <c r="D16" s="46"/>
       <c r="E16" s="3">
         <v>4</v>
       </c>
       <c r="F16" s="3">
         <v>4</v>
       </c>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="14"/>
-      <c r="S16" s="14"/>
-      <c r="T16" s="14"/>
+      <c r="G16" s="3">
+        <v>4</v>
+      </c>
+      <c r="H16" s="3">
+        <v>4</v>
+      </c>
+      <c r="I16" s="3">
+        <v>4</v>
+      </c>
+      <c r="J16" s="3">
+        <v>4</v>
+      </c>
+      <c r="K16" s="3">
+        <v>4</v>
+      </c>
+      <c r="L16" s="3">
+        <v>4</v>
+      </c>
+      <c r="M16" s="3">
+        <v>4</v>
+      </c>
+      <c r="N16" s="3">
+        <v>4</v>
+      </c>
+      <c r="O16" s="3">
+        <v>4</v>
+      </c>
+      <c r="P16" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>4</v>
+      </c>
+      <c r="R16" s="3">
+        <v>4</v>
+      </c>
+      <c r="S16" s="3">
+        <v>4</v>
+      </c>
+      <c r="T16" s="3">
+        <v>4</v>
+      </c>
       <c r="U16" s="14"/>
       <c r="V16" s="15" t="e">
         <f t="shared" si="0"/>
@@ -4197,30 +5394,58 @@
       <c r="B17" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="40" t="s">
+      <c r="C17" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="D17" s="41"/>
+      <c r="D17" s="46"/>
       <c r="E17" s="3">
         <v>3</v>
       </c>
       <c r="F17" s="3">
         <v>3</v>
       </c>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="14"/>
-      <c r="Q17" s="14"/>
-      <c r="R17" s="14"/>
-      <c r="S17" s="14"/>
-      <c r="T17" s="14"/>
+      <c r="G17" s="3">
+        <v>3</v>
+      </c>
+      <c r="H17" s="3">
+        <v>3</v>
+      </c>
+      <c r="I17" s="3">
+        <v>3</v>
+      </c>
+      <c r="J17" s="3">
+        <v>3</v>
+      </c>
+      <c r="K17" s="3">
+        <v>3</v>
+      </c>
+      <c r="L17" s="3">
+        <v>3</v>
+      </c>
+      <c r="M17" s="3">
+        <v>3</v>
+      </c>
+      <c r="N17" s="3">
+        <v>3</v>
+      </c>
+      <c r="O17" s="3">
+        <v>3</v>
+      </c>
+      <c r="P17" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>3</v>
+      </c>
+      <c r="R17" s="3">
+        <v>3</v>
+      </c>
+      <c r="S17" s="3">
+        <v>3</v>
+      </c>
+      <c r="T17" s="3">
+        <v>3</v>
+      </c>
       <c r="U17" s="14"/>
       <c r="V17" s="15" t="e">
         <f t="shared" si="0"/>
@@ -4241,30 +5466,58 @@
       <c r="B18" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="C18" s="40" t="s">
+      <c r="C18" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="D18" s="41"/>
+      <c r="D18" s="46"/>
       <c r="E18" s="3">
         <v>4</v>
       </c>
       <c r="F18" s="3">
         <v>4</v>
       </c>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="14"/>
-      <c r="O18" s="14"/>
-      <c r="P18" s="14"/>
-      <c r="Q18" s="14"/>
-      <c r="R18" s="14"/>
-      <c r="S18" s="14"/>
-      <c r="T18" s="14"/>
+      <c r="G18" s="3">
+        <v>4</v>
+      </c>
+      <c r="H18" s="3">
+        <v>4</v>
+      </c>
+      <c r="I18" s="3">
+        <v>4</v>
+      </c>
+      <c r="J18" s="3">
+        <v>4</v>
+      </c>
+      <c r="K18" s="3">
+        <v>4</v>
+      </c>
+      <c r="L18" s="3">
+        <v>4</v>
+      </c>
+      <c r="M18" s="3">
+        <v>4</v>
+      </c>
+      <c r="N18" s="3">
+        <v>4</v>
+      </c>
+      <c r="O18" s="3">
+        <v>4</v>
+      </c>
+      <c r="P18" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>4</v>
+      </c>
+      <c r="R18" s="3">
+        <v>4</v>
+      </c>
+      <c r="S18" s="3">
+        <v>4</v>
+      </c>
+      <c r="T18" s="3">
+        <v>4</v>
+      </c>
       <c r="U18" s="14"/>
       <c r="V18" s="15" t="e">
         <f t="shared" si="0"/>
@@ -4285,30 +5538,58 @@
       <c r="B19" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="C19" s="40" t="s">
+      <c r="C19" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="D19" s="41"/>
+      <c r="D19" s="46"/>
       <c r="E19" s="3">
         <v>3</v>
       </c>
       <c r="F19" s="3">
         <v>3</v>
       </c>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="14"/>
-      <c r="P19" s="14"/>
-      <c r="Q19" s="14"/>
-      <c r="R19" s="14"/>
-      <c r="S19" s="14"/>
-      <c r="T19" s="14"/>
+      <c r="G19" s="3">
+        <v>3</v>
+      </c>
+      <c r="H19" s="3">
+        <v>3</v>
+      </c>
+      <c r="I19" s="3">
+        <v>3</v>
+      </c>
+      <c r="J19" s="3">
+        <v>3</v>
+      </c>
+      <c r="K19" s="3">
+        <v>3</v>
+      </c>
+      <c r="L19" s="3">
+        <v>3</v>
+      </c>
+      <c r="M19" s="3">
+        <v>3</v>
+      </c>
+      <c r="N19" s="3">
+        <v>3</v>
+      </c>
+      <c r="O19" s="3">
+        <v>3</v>
+      </c>
+      <c r="P19" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>3</v>
+      </c>
+      <c r="R19" s="3">
+        <v>3</v>
+      </c>
+      <c r="S19" s="3">
+        <v>3</v>
+      </c>
+      <c r="T19" s="3">
+        <v>3</v>
+      </c>
       <c r="U19" s="14"/>
       <c r="V19" s="15" t="e">
         <f t="shared" si="0"/>
@@ -4329,30 +5610,58 @@
       <c r="B20" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="40" t="s">
+      <c r="C20" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="D20" s="41"/>
+      <c r="D20" s="46"/>
       <c r="E20" s="3">
         <v>3</v>
       </c>
       <c r="F20" s="3">
         <v>3</v>
       </c>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
-      <c r="P20" s="14"/>
-      <c r="Q20" s="14"/>
-      <c r="R20" s="14"/>
-      <c r="S20" s="14"/>
-      <c r="T20" s="14"/>
+      <c r="G20" s="3">
+        <v>3</v>
+      </c>
+      <c r="H20" s="3">
+        <v>3</v>
+      </c>
+      <c r="I20" s="3">
+        <v>3</v>
+      </c>
+      <c r="J20" s="3">
+        <v>3</v>
+      </c>
+      <c r="K20" s="3">
+        <v>3</v>
+      </c>
+      <c r="L20" s="3">
+        <v>3</v>
+      </c>
+      <c r="M20" s="3">
+        <v>3</v>
+      </c>
+      <c r="N20" s="3">
+        <v>3</v>
+      </c>
+      <c r="O20" s="3">
+        <v>3</v>
+      </c>
+      <c r="P20" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>3</v>
+      </c>
+      <c r="R20" s="3">
+        <v>3</v>
+      </c>
+      <c r="S20" s="3">
+        <v>3</v>
+      </c>
+      <c r="T20" s="3">
+        <v>3</v>
+      </c>
       <c r="U20" s="14"/>
       <c r="V20" s="15" t="e">
         <f t="shared" si="0"/>
@@ -4373,30 +5682,58 @@
       <c r="B21" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="C21" s="40" t="s">
+      <c r="C21" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="D21" s="41"/>
+      <c r="D21" s="46"/>
       <c r="E21" s="3">
         <v>3</v>
       </c>
       <c r="F21" s="3">
         <v>3</v>
       </c>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
-      <c r="P21" s="14"/>
-      <c r="Q21" s="14"/>
-      <c r="R21" s="14"/>
-      <c r="S21" s="14"/>
-      <c r="T21" s="14"/>
+      <c r="G21" s="3">
+        <v>3</v>
+      </c>
+      <c r="H21" s="3">
+        <v>3</v>
+      </c>
+      <c r="I21" s="3">
+        <v>3</v>
+      </c>
+      <c r="J21" s="3">
+        <v>3</v>
+      </c>
+      <c r="K21" s="3">
+        <v>3</v>
+      </c>
+      <c r="L21" s="3">
+        <v>3</v>
+      </c>
+      <c r="M21" s="3">
+        <v>3</v>
+      </c>
+      <c r="N21" s="3">
+        <v>3</v>
+      </c>
+      <c r="O21" s="3">
+        <v>3</v>
+      </c>
+      <c r="P21" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>3</v>
+      </c>
+      <c r="R21" s="3">
+        <v>3</v>
+      </c>
+      <c r="S21" s="3">
+        <v>3</v>
+      </c>
+      <c r="T21" s="3">
+        <v>3</v>
+      </c>
       <c r="U21" s="14"/>
       <c r="V21" s="15" t="e">
         <f t="shared" si="0"/>
@@ -4417,30 +5754,58 @@
       <c r="B22" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="C22" s="40" t="s">
+      <c r="C22" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="D22" s="41"/>
+      <c r="D22" s="46"/>
       <c r="E22" s="3">
         <v>4</v>
       </c>
       <c r="F22" s="3">
         <v>4</v>
       </c>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="14"/>
-      <c r="O22" s="14"/>
-      <c r="P22" s="14"/>
-      <c r="Q22" s="14"/>
-      <c r="R22" s="14"/>
-      <c r="S22" s="14"/>
-      <c r="T22" s="14"/>
+      <c r="G22" s="3">
+        <v>4</v>
+      </c>
+      <c r="H22" s="3">
+        <v>4</v>
+      </c>
+      <c r="I22" s="3">
+        <v>4</v>
+      </c>
+      <c r="J22" s="3">
+        <v>4</v>
+      </c>
+      <c r="K22" s="3">
+        <v>4</v>
+      </c>
+      <c r="L22" s="3">
+        <v>4</v>
+      </c>
+      <c r="M22" s="3">
+        <v>4</v>
+      </c>
+      <c r="N22" s="3">
+        <v>4</v>
+      </c>
+      <c r="O22" s="3">
+        <v>4</v>
+      </c>
+      <c r="P22" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>4</v>
+      </c>
+      <c r="R22" s="3">
+        <v>4</v>
+      </c>
+      <c r="S22" s="3">
+        <v>4</v>
+      </c>
+      <c r="T22" s="3">
+        <v>4</v>
+      </c>
       <c r="U22" s="14"/>
       <c r="V22" s="15" t="e">
         <f t="shared" si="0"/>
@@ -4461,30 +5826,58 @@
       <c r="B23" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="C23" s="40" t="s">
+      <c r="C23" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="D23" s="41"/>
+      <c r="D23" s="46"/>
       <c r="E23" s="3">
         <v>4</v>
       </c>
       <c r="F23" s="3">
         <v>4</v>
       </c>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
-      <c r="N23" s="18"/>
-      <c r="O23" s="18"/>
-      <c r="P23" s="18"/>
-      <c r="Q23" s="18"/>
-      <c r="R23" s="18"/>
-      <c r="S23" s="18"/>
-      <c r="T23" s="18"/>
+      <c r="G23" s="3">
+        <v>4</v>
+      </c>
+      <c r="H23" s="3">
+        <v>4</v>
+      </c>
+      <c r="I23" s="3">
+        <v>4</v>
+      </c>
+      <c r="J23" s="3">
+        <v>4</v>
+      </c>
+      <c r="K23" s="3">
+        <v>4</v>
+      </c>
+      <c r="L23" s="3">
+        <v>4</v>
+      </c>
+      <c r="M23" s="3">
+        <v>4</v>
+      </c>
+      <c r="N23" s="3">
+        <v>4</v>
+      </c>
+      <c r="O23" s="3">
+        <v>4</v>
+      </c>
+      <c r="P23" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>4</v>
+      </c>
+      <c r="R23" s="3">
+        <v>4</v>
+      </c>
+      <c r="S23" s="3">
+        <v>4</v>
+      </c>
+      <c r="T23" s="3">
+        <v>4</v>
+      </c>
       <c r="U23" s="18"/>
       <c r="V23" s="15" t="e">
         <f t="shared" si="0"/>
@@ -4505,14 +5898,56 @@
       <c r="B24" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="C24" s="42" t="s">
+      <c r="C24" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="D24" s="43"/>
+      <c r="D24" s="48"/>
       <c r="E24" s="3">
         <v>3</v>
       </c>
       <c r="F24" s="3">
+        <v>3</v>
+      </c>
+      <c r="G24" s="3">
+        <v>3</v>
+      </c>
+      <c r="H24" s="3">
+        <v>3</v>
+      </c>
+      <c r="I24" s="3">
+        <v>3</v>
+      </c>
+      <c r="J24" s="3">
+        <v>3</v>
+      </c>
+      <c r="K24" s="3">
+        <v>3</v>
+      </c>
+      <c r="L24" s="3">
+        <v>3</v>
+      </c>
+      <c r="M24" s="3">
+        <v>3</v>
+      </c>
+      <c r="N24" s="3">
+        <v>3</v>
+      </c>
+      <c r="O24" s="3">
+        <v>3</v>
+      </c>
+      <c r="P24" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>3</v>
+      </c>
+      <c r="R24" s="3">
+        <v>3</v>
+      </c>
+      <c r="S24" s="3">
+        <v>3</v>
+      </c>
+      <c r="T24" s="3">
         <v>3</v>
       </c>
       <c r="V24" s="15" t="e">
@@ -4534,14 +5969,56 @@
       <c r="B25" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="C25" s="42" t="s">
+      <c r="C25" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="D25" s="43"/>
+      <c r="D25" s="48"/>
       <c r="E25" s="3">
         <v>4</v>
       </c>
       <c r="F25" s="3">
+        <v>4</v>
+      </c>
+      <c r="G25" s="3">
+        <v>4</v>
+      </c>
+      <c r="H25" s="3">
+        <v>4</v>
+      </c>
+      <c r="I25" s="3">
+        <v>4</v>
+      </c>
+      <c r="J25" s="3">
+        <v>4</v>
+      </c>
+      <c r="K25" s="3">
+        <v>4</v>
+      </c>
+      <c r="L25" s="3">
+        <v>4</v>
+      </c>
+      <c r="M25" s="3">
+        <v>4</v>
+      </c>
+      <c r="N25" s="3">
+        <v>4</v>
+      </c>
+      <c r="O25" s="3">
+        <v>4</v>
+      </c>
+      <c r="P25" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q25" s="3">
+        <v>4</v>
+      </c>
+      <c r="R25" s="3">
+        <v>4</v>
+      </c>
+      <c r="S25" s="3">
+        <v>4</v>
+      </c>
+      <c r="T25" s="3">
         <v>4</v>
       </c>
       <c r="V25" s="15" t="e">
@@ -4563,14 +6040,56 @@
       <c r="B26" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="C26" s="40" t="s">
+      <c r="C26" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="D26" s="41"/>
+      <c r="D26" s="46"/>
       <c r="E26" s="3">
         <v>4</v>
       </c>
       <c r="F26" s="3">
+        <v>4</v>
+      </c>
+      <c r="G26" s="3">
+        <v>4</v>
+      </c>
+      <c r="H26" s="3">
+        <v>4</v>
+      </c>
+      <c r="I26" s="3">
+        <v>4</v>
+      </c>
+      <c r="J26" s="3">
+        <v>4</v>
+      </c>
+      <c r="K26" s="3">
+        <v>4</v>
+      </c>
+      <c r="L26" s="3">
+        <v>4</v>
+      </c>
+      <c r="M26" s="3">
+        <v>4</v>
+      </c>
+      <c r="N26" s="3">
+        <v>4</v>
+      </c>
+      <c r="O26" s="3">
+        <v>4</v>
+      </c>
+      <c r="P26" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q26" s="3">
+        <v>4</v>
+      </c>
+      <c r="R26" s="3">
+        <v>4</v>
+      </c>
+      <c r="S26" s="3">
+        <v>4</v>
+      </c>
+      <c r="T26" s="3">
         <v>4</v>
       </c>
       <c r="V26" s="15" t="e">
@@ -4592,14 +6111,56 @@
       <c r="B27" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="C27" s="42" t="s">
+      <c r="C27" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="D27" s="43"/>
+      <c r="D27" s="48"/>
       <c r="E27" s="3">
         <v>4</v>
       </c>
       <c r="F27" s="3">
+        <v>4</v>
+      </c>
+      <c r="G27" s="3">
+        <v>4</v>
+      </c>
+      <c r="H27" s="3">
+        <v>4</v>
+      </c>
+      <c r="I27" s="3">
+        <v>4</v>
+      </c>
+      <c r="J27" s="3">
+        <v>4</v>
+      </c>
+      <c r="K27" s="3">
+        <v>4</v>
+      </c>
+      <c r="L27" s="3">
+        <v>4</v>
+      </c>
+      <c r="M27" s="3">
+        <v>4</v>
+      </c>
+      <c r="N27" s="3">
+        <v>4</v>
+      </c>
+      <c r="O27" s="3">
+        <v>4</v>
+      </c>
+      <c r="P27" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q27" s="3">
+        <v>4</v>
+      </c>
+      <c r="R27" s="3">
+        <v>4</v>
+      </c>
+      <c r="S27" s="3">
+        <v>4</v>
+      </c>
+      <c r="T27" s="3">
         <v>4</v>
       </c>
       <c r="V27" s="15" t="e">
@@ -4615,11 +6176,11 @@
       </c>
     </row>
     <row r="28" spans="2:24" customFormat="false">
-      <c r="B28" s="39" t="s">
+      <c r="B28" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="39"/>
-      <c r="D28" s="39"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="44"/>
       <c r="E28" s="3">
         <f>SUM(E3:E27)</f>
         <v>0</v>
@@ -4698,70 +6259,70 @@
       <c r="B30" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="45" t="s">
+      <c r="C30" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="D30" s="45"/>
+      <c r="D30" s="50"/>
       <c r="E30" s="22"/>
     </row>
     <row r="31" spans="2:5" customFormat="false" ht="51.75" customHeight="1">
       <c r="B31" s="11">
         <v>5</v>
       </c>
-      <c r="C31" s="46" t="s">
+      <c r="C31" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="D31" s="46"/>
+      <c r="D31" s="51"/>
       <c r="E31" s="24"/>
     </row>
     <row r="32" spans="2:5" customFormat="false" ht="33.75" customHeight="1">
       <c r="B32" s="11">
         <v>4</v>
       </c>
-      <c r="C32" s="44" t="s">
+      <c r="C32" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="D32" s="44"/>
+      <c r="D32" s="49"/>
       <c r="E32" s="24"/>
     </row>
     <row r="33" spans="2:5" customFormat="false" ht="30" customHeight="1">
       <c r="B33" s="11">
         <v>3</v>
       </c>
-      <c r="C33" s="44" t="s">
+      <c r="C33" s="49" t="s">
         <v>79</v>
       </c>
-      <c r="D33" s="44"/>
+      <c r="D33" s="49"/>
       <c r="E33" s="24"/>
     </row>
     <row r="34" spans="2:5" customFormat="false" ht="31.5" customHeight="1">
       <c r="B34" s="11">
         <v>2</v>
       </c>
-      <c r="C34" s="44" t="s">
+      <c r="C34" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="D34" s="44"/>
+      <c r="D34" s="49"/>
       <c r="E34" s="24"/>
     </row>
     <row r="35" spans="2:5" customFormat="false" ht="39" customHeight="1">
       <c r="B35" s="11">
         <v>1</v>
       </c>
-      <c r="C35" s="44" t="s">
+      <c r="C35" s="49" t="s">
         <v>81</v>
       </c>
-      <c r="D35" s="44"/>
+      <c r="D35" s="49"/>
       <c r="E35" s="24"/>
     </row>
     <row r="36" spans="2:5" customFormat="false" ht="36.75" customHeight="1">
       <c r="B36" s="11">
         <v>0</v>
       </c>
-      <c r="C36" s="44" t="s">
+      <c r="C36" s="49" t="s">
         <v>82</v>
       </c>
-      <c r="D36" s="44"/>
+      <c r="D36" s="49"/>
       <c r="E36" s="24"/>
     </row>
   </sheetData>
@@ -4810,13 +6371,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:X32"/>
+  <dimension ref="A1:Y32"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="E13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2:U2"/>
+      <selection pane="bottomRight" activeCell="Y3" sqref="Y3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4831,7 +6392,8 @@
     <col min="22" max="22" width="8.7109375" style="5" customWidth="1"/>
     <col min="23" max="23" width="10.28515625" style="3" customWidth="1"/>
     <col min="24" max="24" width="9.85546875" style="3" customWidth="1"/>
-    <col min="25" max="16384" width="9.140625" style="3"/>
+    <col min="25" max="25" width="24.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" customFormat="false" ht="33.75">
@@ -4845,7 +6407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="3:24" s="6" customFormat="1" ht="90">
+    <row r="2" spans="3:25" s="6" customFormat="1" ht="90">
       <c r="C2" s="7"/>
       <c r="E2" s="8" t="s">
         <v>116</v>
@@ -4853,62 +6415,65 @@
       <c r="F2" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="39" t="s">
         <v>118</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="39" t="s">
         <v>120</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="J2" s="39" t="s">
         <v>121</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="K2" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="M2" s="17" t="s">
+      <c r="M2" s="39" t="s">
         <v>124</v>
       </c>
-      <c r="N2" s="17" t="s">
+      <c r="N2" s="39" t="s">
         <v>125</v>
       </c>
-      <c r="O2" s="17" t="s">
+      <c r="O2" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="P2" s="17" t="s">
+      <c r="P2" s="39" t="s">
         <v>127</v>
       </c>
-      <c r="Q2" s="17" t="s">
+      <c r="Q2" s="39" t="s">
         <v>128</v>
       </c>
-      <c r="R2" s="17" t="s">
+      <c r="R2" s="39" t="s">
         <v>129</v>
       </c>
-      <c r="S2" s="17" t="s">
+      <c r="S2" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="T2" s="17" t="s">
+      <c r="T2" s="39" t="s">
         <v>131</v>
       </c>
-      <c r="U2" s="17" t="s">
+      <c r="U2" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="V2" s="9" t="s">
+      <c r="V2" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="W2" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="X2" s="10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" s="14" customFormat="1" ht="31.5">
+      <c r="W2" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="X2" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y2" s="41" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" s="14" customFormat="1" ht="31.5">
       <c r="A3" s="31" t="s">
         <v>85</v>
       </c>
@@ -4924,7 +6489,49 @@
       <c r="E3" s="14">
         <v>4</v>
       </c>
+      <c r="F3" s="14">
+        <v>4</v>
+      </c>
+      <c r="G3" s="14">
+        <v>4</v>
+      </c>
       <c r="H3" s="14">
+        <v>4</v>
+      </c>
+      <c r="I3" s="14">
+        <v>4</v>
+      </c>
+      <c r="J3" s="14">
+        <v>4</v>
+      </c>
+      <c r="K3" s="14">
+        <v>4</v>
+      </c>
+      <c r="L3" s="14">
+        <v>4</v>
+      </c>
+      <c r="M3" s="14">
+        <v>4</v>
+      </c>
+      <c r="N3" s="14">
+        <v>4</v>
+      </c>
+      <c r="O3" s="14">
+        <v>4</v>
+      </c>
+      <c r="P3" s="14">
+        <v>4</v>
+      </c>
+      <c r="Q3" s="14">
+        <v>4</v>
+      </c>
+      <c r="R3" s="14">
+        <v>4</v>
+      </c>
+      <c r="S3" s="14">
+        <v>4</v>
+      </c>
+      <c r="T3" s="14">
         <v>4</v>
       </c>
       <c r="V3" s="15" t="e">
@@ -4936,6 +6543,10 @@
       </c>
       <c r="X3" s="16" t="e">
         <f>V3*W3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y3" s="40" t="e">
+        <f>SUM(X24, '熱意- nhiet_tinh'!X28, '考え方- tu_duy'!W28)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -4955,7 +6566,49 @@
       <c r="E4" s="14">
         <v>4</v>
       </c>
+      <c r="F4" s="14">
+        <v>4</v>
+      </c>
+      <c r="G4" s="14">
+        <v>4</v>
+      </c>
       <c r="H4" s="14">
+        <v>4</v>
+      </c>
+      <c r="I4" s="14">
+        <v>4</v>
+      </c>
+      <c r="J4" s="14">
+        <v>4</v>
+      </c>
+      <c r="K4" s="14">
+        <v>4</v>
+      </c>
+      <c r="L4" s="14">
+        <v>4</v>
+      </c>
+      <c r="M4" s="14">
+        <v>4</v>
+      </c>
+      <c r="N4" s="14">
+        <v>4</v>
+      </c>
+      <c r="O4" s="14">
+        <v>4</v>
+      </c>
+      <c r="P4" s="14">
+        <v>4</v>
+      </c>
+      <c r="Q4" s="14">
+        <v>4</v>
+      </c>
+      <c r="R4" s="14">
+        <v>4</v>
+      </c>
+      <c r="S4" s="14">
+        <v>4</v>
+      </c>
+      <c r="T4" s="14">
         <v>4</v>
       </c>
       <c r="V4" s="15" t="e">
@@ -4986,7 +6639,49 @@
       <c r="E5" s="14">
         <v>3</v>
       </c>
+      <c r="F5" s="14">
+        <v>3</v>
+      </c>
+      <c r="G5" s="14">
+        <v>3</v>
+      </c>
       <c r="H5" s="14">
+        <v>3</v>
+      </c>
+      <c r="I5" s="14">
+        <v>3</v>
+      </c>
+      <c r="J5" s="14">
+        <v>3</v>
+      </c>
+      <c r="K5" s="14">
+        <v>3</v>
+      </c>
+      <c r="L5" s="14">
+        <v>3</v>
+      </c>
+      <c r="M5" s="14">
+        <v>3</v>
+      </c>
+      <c r="N5" s="14">
+        <v>3</v>
+      </c>
+      <c r="O5" s="14">
+        <v>3</v>
+      </c>
+      <c r="P5" s="14">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="14">
+        <v>3</v>
+      </c>
+      <c r="R5" s="14">
+        <v>3</v>
+      </c>
+      <c r="S5" s="14">
+        <v>3</v>
+      </c>
+      <c r="T5" s="14">
         <v>3</v>
       </c>
       <c r="V5" s="15" t="e">
@@ -5017,7 +6712,49 @@
       <c r="E6" s="14">
         <v>3</v>
       </c>
+      <c r="F6" s="14">
+        <v>3</v>
+      </c>
+      <c r="G6" s="14">
+        <v>3</v>
+      </c>
       <c r="H6" s="14">
+        <v>3</v>
+      </c>
+      <c r="I6" s="14">
+        <v>3</v>
+      </c>
+      <c r="J6" s="14">
+        <v>3</v>
+      </c>
+      <c r="K6" s="14">
+        <v>3</v>
+      </c>
+      <c r="L6" s="14">
+        <v>3</v>
+      </c>
+      <c r="M6" s="14">
+        <v>3</v>
+      </c>
+      <c r="N6" s="14">
+        <v>3</v>
+      </c>
+      <c r="O6" s="14">
+        <v>3</v>
+      </c>
+      <c r="P6" s="14">
+        <v>3</v>
+      </c>
+      <c r="Q6" s="14">
+        <v>3</v>
+      </c>
+      <c r="R6" s="14">
+        <v>3</v>
+      </c>
+      <c r="S6" s="14">
+        <v>3</v>
+      </c>
+      <c r="T6" s="14">
         <v>3</v>
       </c>
       <c r="V6" s="15" t="e">
@@ -5048,7 +6785,49 @@
       <c r="E7" s="14">
         <v>3</v>
       </c>
+      <c r="F7" s="14">
+        <v>3</v>
+      </c>
+      <c r="G7" s="14">
+        <v>3</v>
+      </c>
       <c r="H7" s="14">
+        <v>3</v>
+      </c>
+      <c r="I7" s="14">
+        <v>3</v>
+      </c>
+      <c r="J7" s="14">
+        <v>3</v>
+      </c>
+      <c r="K7" s="14">
+        <v>3</v>
+      </c>
+      <c r="L7" s="14">
+        <v>3</v>
+      </c>
+      <c r="M7" s="14">
+        <v>3</v>
+      </c>
+      <c r="N7" s="14">
+        <v>3</v>
+      </c>
+      <c r="O7" s="14">
+        <v>3</v>
+      </c>
+      <c r="P7" s="14">
+        <v>3</v>
+      </c>
+      <c r="Q7" s="14">
+        <v>3</v>
+      </c>
+      <c r="R7" s="14">
+        <v>3</v>
+      </c>
+      <c r="S7" s="14">
+        <v>3</v>
+      </c>
+      <c r="T7" s="14">
         <v>3</v>
       </c>
       <c r="V7" s="15" t="e">
@@ -5079,7 +6858,49 @@
       <c r="E8" s="14">
         <v>4</v>
       </c>
+      <c r="F8" s="14">
+        <v>4</v>
+      </c>
+      <c r="G8" s="14">
+        <v>4</v>
+      </c>
       <c r="H8" s="14">
+        <v>4</v>
+      </c>
+      <c r="I8" s="14">
+        <v>4</v>
+      </c>
+      <c r="J8" s="14">
+        <v>4</v>
+      </c>
+      <c r="K8" s="14">
+        <v>4</v>
+      </c>
+      <c r="L8" s="14">
+        <v>4</v>
+      </c>
+      <c r="M8" s="14">
+        <v>4</v>
+      </c>
+      <c r="N8" s="14">
+        <v>4</v>
+      </c>
+      <c r="O8" s="14">
+        <v>4</v>
+      </c>
+      <c r="P8" s="14">
+        <v>4</v>
+      </c>
+      <c r="Q8" s="14">
+        <v>4</v>
+      </c>
+      <c r="R8" s="14">
+        <v>4</v>
+      </c>
+      <c r="S8" s="14">
+        <v>4</v>
+      </c>
+      <c r="T8" s="14">
         <v>4</v>
       </c>
       <c r="V8" s="15" t="e">
@@ -5110,7 +6931,49 @@
       <c r="E9" s="14">
         <v>4</v>
       </c>
+      <c r="F9" s="14">
+        <v>4</v>
+      </c>
+      <c r="G9" s="14">
+        <v>4</v>
+      </c>
       <c r="H9" s="14">
+        <v>4</v>
+      </c>
+      <c r="I9" s="14">
+        <v>4</v>
+      </c>
+      <c r="J9" s="14">
+        <v>4</v>
+      </c>
+      <c r="K9" s="14">
+        <v>4</v>
+      </c>
+      <c r="L9" s="14">
+        <v>4</v>
+      </c>
+      <c r="M9" s="14">
+        <v>4</v>
+      </c>
+      <c r="N9" s="14">
+        <v>4</v>
+      </c>
+      <c r="O9" s="14">
+        <v>4</v>
+      </c>
+      <c r="P9" s="14">
+        <v>4</v>
+      </c>
+      <c r="Q9" s="14">
+        <v>4</v>
+      </c>
+      <c r="R9" s="14">
+        <v>4</v>
+      </c>
+      <c r="S9" s="14">
+        <v>4</v>
+      </c>
+      <c r="T9" s="14">
         <v>4</v>
       </c>
       <c r="V9" s="15" t="e">
@@ -5141,7 +7004,49 @@
       <c r="E10" s="14">
         <v>4</v>
       </c>
+      <c r="F10" s="14">
+        <v>4</v>
+      </c>
+      <c r="G10" s="14">
+        <v>4</v>
+      </c>
       <c r="H10" s="14">
+        <v>4</v>
+      </c>
+      <c r="I10" s="14">
+        <v>4</v>
+      </c>
+      <c r="J10" s="14">
+        <v>4</v>
+      </c>
+      <c r="K10" s="14">
+        <v>4</v>
+      </c>
+      <c r="L10" s="14">
+        <v>4</v>
+      </c>
+      <c r="M10" s="14">
+        <v>4</v>
+      </c>
+      <c r="N10" s="14">
+        <v>4</v>
+      </c>
+      <c r="O10" s="14">
+        <v>4</v>
+      </c>
+      <c r="P10" s="14">
+        <v>4</v>
+      </c>
+      <c r="Q10" s="14">
+        <v>4</v>
+      </c>
+      <c r="R10" s="14">
+        <v>4</v>
+      </c>
+      <c r="S10" s="14">
+        <v>4</v>
+      </c>
+      <c r="T10" s="14">
         <v>4</v>
       </c>
       <c r="V10" s="15" t="e">
@@ -5172,7 +7077,49 @@
       <c r="E11" s="14">
         <v>3</v>
       </c>
+      <c r="F11" s="14">
+        <v>3</v>
+      </c>
+      <c r="G11" s="14">
+        <v>3</v>
+      </c>
       <c r="H11" s="14">
+        <v>3</v>
+      </c>
+      <c r="I11" s="14">
+        <v>3</v>
+      </c>
+      <c r="J11" s="14">
+        <v>3</v>
+      </c>
+      <c r="K11" s="14">
+        <v>3</v>
+      </c>
+      <c r="L11" s="14">
+        <v>3</v>
+      </c>
+      <c r="M11" s="14">
+        <v>3</v>
+      </c>
+      <c r="N11" s="14">
+        <v>3</v>
+      </c>
+      <c r="O11" s="14">
+        <v>3</v>
+      </c>
+      <c r="P11" s="14">
+        <v>3</v>
+      </c>
+      <c r="Q11" s="14">
+        <v>3</v>
+      </c>
+      <c r="R11" s="14">
+        <v>3</v>
+      </c>
+      <c r="S11" s="14">
+        <v>3</v>
+      </c>
+      <c r="T11" s="14">
         <v>3</v>
       </c>
       <c r="V11" s="15" t="e">
@@ -5203,7 +7150,49 @@
       <c r="E12" s="14">
         <v>4</v>
       </c>
+      <c r="F12" s="14">
+        <v>4</v>
+      </c>
+      <c r="G12" s="14">
+        <v>4</v>
+      </c>
       <c r="H12" s="14">
+        <v>4</v>
+      </c>
+      <c r="I12" s="14">
+        <v>4</v>
+      </c>
+      <c r="J12" s="14">
+        <v>4</v>
+      </c>
+      <c r="K12" s="14">
+        <v>4</v>
+      </c>
+      <c r="L12" s="14">
+        <v>4</v>
+      </c>
+      <c r="M12" s="14">
+        <v>4</v>
+      </c>
+      <c r="N12" s="14">
+        <v>4</v>
+      </c>
+      <c r="O12" s="14">
+        <v>4</v>
+      </c>
+      <c r="P12" s="14">
+        <v>4</v>
+      </c>
+      <c r="Q12" s="14">
+        <v>4</v>
+      </c>
+      <c r="R12" s="14">
+        <v>4</v>
+      </c>
+      <c r="S12" s="14">
+        <v>4</v>
+      </c>
+      <c r="T12" s="14">
         <v>4</v>
       </c>
       <c r="V12" s="15" t="e">
@@ -5234,7 +7223,49 @@
       <c r="E13" s="14">
         <v>4</v>
       </c>
+      <c r="F13" s="14">
+        <v>4</v>
+      </c>
+      <c r="G13" s="14">
+        <v>4</v>
+      </c>
       <c r="H13" s="14">
+        <v>4</v>
+      </c>
+      <c r="I13" s="14">
+        <v>4</v>
+      </c>
+      <c r="J13" s="14">
+        <v>4</v>
+      </c>
+      <c r="K13" s="14">
+        <v>4</v>
+      </c>
+      <c r="L13" s="14">
+        <v>4</v>
+      </c>
+      <c r="M13" s="14">
+        <v>4</v>
+      </c>
+      <c r="N13" s="14">
+        <v>4</v>
+      </c>
+      <c r="O13" s="14">
+        <v>4</v>
+      </c>
+      <c r="P13" s="14">
+        <v>4</v>
+      </c>
+      <c r="Q13" s="14">
+        <v>4</v>
+      </c>
+      <c r="R13" s="14">
+        <v>4</v>
+      </c>
+      <c r="S13" s="14">
+        <v>4</v>
+      </c>
+      <c r="T13" s="14">
         <v>4</v>
       </c>
       <c r="V13" s="15" t="e">
@@ -5265,7 +7296,49 @@
       <c r="E14" s="14">
         <v>4</v>
       </c>
+      <c r="F14" s="14">
+        <v>4</v>
+      </c>
+      <c r="G14" s="14">
+        <v>4</v>
+      </c>
       <c r="H14" s="14">
+        <v>4</v>
+      </c>
+      <c r="I14" s="14">
+        <v>4</v>
+      </c>
+      <c r="J14" s="14">
+        <v>4</v>
+      </c>
+      <c r="K14" s="14">
+        <v>4</v>
+      </c>
+      <c r="L14" s="14">
+        <v>4</v>
+      </c>
+      <c r="M14" s="14">
+        <v>4</v>
+      </c>
+      <c r="N14" s="14">
+        <v>4</v>
+      </c>
+      <c r="O14" s="14">
+        <v>4</v>
+      </c>
+      <c r="P14" s="14">
+        <v>4</v>
+      </c>
+      <c r="Q14" s="14">
+        <v>4</v>
+      </c>
+      <c r="R14" s="14">
+        <v>4</v>
+      </c>
+      <c r="S14" s="14">
+        <v>4</v>
+      </c>
+      <c r="T14" s="14">
         <v>4</v>
       </c>
       <c r="V14" s="15" t="e">
@@ -5296,7 +7369,49 @@
       <c r="E15" s="14">
         <v>4</v>
       </c>
+      <c r="F15" s="14">
+        <v>4</v>
+      </c>
+      <c r="G15" s="14">
+        <v>4</v>
+      </c>
       <c r="H15" s="14">
+        <v>4</v>
+      </c>
+      <c r="I15" s="14">
+        <v>4</v>
+      </c>
+      <c r="J15" s="14">
+        <v>4</v>
+      </c>
+      <c r="K15" s="14">
+        <v>4</v>
+      </c>
+      <c r="L15" s="14">
+        <v>4</v>
+      </c>
+      <c r="M15" s="14">
+        <v>4</v>
+      </c>
+      <c r="N15" s="14">
+        <v>4</v>
+      </c>
+      <c r="O15" s="14">
+        <v>4</v>
+      </c>
+      <c r="P15" s="14">
+        <v>4</v>
+      </c>
+      <c r="Q15" s="14">
+        <v>4</v>
+      </c>
+      <c r="R15" s="14">
+        <v>4</v>
+      </c>
+      <c r="S15" s="14">
+        <v>4</v>
+      </c>
+      <c r="T15" s="14">
         <v>4</v>
       </c>
       <c r="V15" s="15" t="e">
@@ -5327,7 +7442,49 @@
       <c r="E16" s="14">
         <v>4</v>
       </c>
+      <c r="F16" s="14">
+        <v>4</v>
+      </c>
+      <c r="G16" s="14">
+        <v>4</v>
+      </c>
       <c r="H16" s="14">
+        <v>4</v>
+      </c>
+      <c r="I16" s="14">
+        <v>4</v>
+      </c>
+      <c r="J16" s="14">
+        <v>4</v>
+      </c>
+      <c r="K16" s="14">
+        <v>4</v>
+      </c>
+      <c r="L16" s="14">
+        <v>4</v>
+      </c>
+      <c r="M16" s="14">
+        <v>4</v>
+      </c>
+      <c r="N16" s="14">
+        <v>4</v>
+      </c>
+      <c r="O16" s="14">
+        <v>4</v>
+      </c>
+      <c r="P16" s="14">
+        <v>4</v>
+      </c>
+      <c r="Q16" s="14">
+        <v>4</v>
+      </c>
+      <c r="R16" s="14">
+        <v>4</v>
+      </c>
+      <c r="S16" s="14">
+        <v>4</v>
+      </c>
+      <c r="T16" s="14">
         <v>4</v>
       </c>
       <c r="V16" s="15" t="e">
@@ -5358,7 +7515,49 @@
       <c r="E17" s="14">
         <v>4</v>
       </c>
+      <c r="F17" s="14">
+        <v>4</v>
+      </c>
+      <c r="G17" s="14">
+        <v>4</v>
+      </c>
       <c r="H17" s="14">
+        <v>4</v>
+      </c>
+      <c r="I17" s="14">
+        <v>4</v>
+      </c>
+      <c r="J17" s="14">
+        <v>4</v>
+      </c>
+      <c r="K17" s="14">
+        <v>4</v>
+      </c>
+      <c r="L17" s="14">
+        <v>4</v>
+      </c>
+      <c r="M17" s="14">
+        <v>4</v>
+      </c>
+      <c r="N17" s="14">
+        <v>4</v>
+      </c>
+      <c r="O17" s="14">
+        <v>4</v>
+      </c>
+      <c r="P17" s="14">
+        <v>4</v>
+      </c>
+      <c r="Q17" s="14">
+        <v>4</v>
+      </c>
+      <c r="R17" s="14">
+        <v>4</v>
+      </c>
+      <c r="S17" s="14">
+        <v>4</v>
+      </c>
+      <c r="T17" s="14">
         <v>4</v>
       </c>
       <c r="V17" s="15" t="e">
@@ -5389,7 +7588,49 @@
       <c r="E18" s="14">
         <v>4</v>
       </c>
+      <c r="F18" s="14">
+        <v>4</v>
+      </c>
+      <c r="G18" s="14">
+        <v>4</v>
+      </c>
       <c r="H18" s="14">
+        <v>4</v>
+      </c>
+      <c r="I18" s="14">
+        <v>4</v>
+      </c>
+      <c r="J18" s="14">
+        <v>4</v>
+      </c>
+      <c r="K18" s="14">
+        <v>4</v>
+      </c>
+      <c r="L18" s="14">
+        <v>4</v>
+      </c>
+      <c r="M18" s="14">
+        <v>4</v>
+      </c>
+      <c r="N18" s="14">
+        <v>4</v>
+      </c>
+      <c r="O18" s="14">
+        <v>4</v>
+      </c>
+      <c r="P18" s="14">
+        <v>4</v>
+      </c>
+      <c r="Q18" s="14">
+        <v>4</v>
+      </c>
+      <c r="R18" s="14">
+        <v>4</v>
+      </c>
+      <c r="S18" s="14">
+        <v>4</v>
+      </c>
+      <c r="T18" s="14">
         <v>4</v>
       </c>
       <c r="V18" s="15" t="e">
@@ -5420,7 +7661,49 @@
       <c r="E19" s="14">
         <v>3</v>
       </c>
+      <c r="F19" s="14">
+        <v>3</v>
+      </c>
+      <c r="G19" s="14">
+        <v>3</v>
+      </c>
       <c r="H19" s="14">
+        <v>3</v>
+      </c>
+      <c r="I19" s="14">
+        <v>3</v>
+      </c>
+      <c r="J19" s="14">
+        <v>3</v>
+      </c>
+      <c r="K19" s="14">
+        <v>3</v>
+      </c>
+      <c r="L19" s="14">
+        <v>3</v>
+      </c>
+      <c r="M19" s="14">
+        <v>3</v>
+      </c>
+      <c r="N19" s="14">
+        <v>3</v>
+      </c>
+      <c r="O19" s="14">
+        <v>3</v>
+      </c>
+      <c r="P19" s="14">
+        <v>3</v>
+      </c>
+      <c r="Q19" s="14">
+        <v>3</v>
+      </c>
+      <c r="R19" s="14">
+        <v>3</v>
+      </c>
+      <c r="S19" s="14">
+        <v>3</v>
+      </c>
+      <c r="T19" s="14">
         <v>3</v>
       </c>
       <c r="V19" s="15" t="e">
@@ -5451,7 +7734,49 @@
       <c r="E20" s="14">
         <v>4</v>
       </c>
+      <c r="F20" s="14">
+        <v>4</v>
+      </c>
+      <c r="G20" s="14">
+        <v>4</v>
+      </c>
       <c r="H20" s="14">
+        <v>4</v>
+      </c>
+      <c r="I20" s="14">
+        <v>4</v>
+      </c>
+      <c r="J20" s="14">
+        <v>4</v>
+      </c>
+      <c r="K20" s="14">
+        <v>4</v>
+      </c>
+      <c r="L20" s="14">
+        <v>4</v>
+      </c>
+      <c r="M20" s="14">
+        <v>4</v>
+      </c>
+      <c r="N20" s="14">
+        <v>4</v>
+      </c>
+      <c r="O20" s="14">
+        <v>4</v>
+      </c>
+      <c r="P20" s="14">
+        <v>4</v>
+      </c>
+      <c r="Q20" s="14">
+        <v>4</v>
+      </c>
+      <c r="R20" s="14">
+        <v>4</v>
+      </c>
+      <c r="S20" s="14">
+        <v>4</v>
+      </c>
+      <c r="T20" s="14">
         <v>4</v>
       </c>
       <c r="V20" s="15" t="e">
@@ -5482,7 +7807,49 @@
       <c r="E21" s="14">
         <v>4</v>
       </c>
+      <c r="F21" s="14">
+        <v>4</v>
+      </c>
+      <c r="G21" s="14">
+        <v>4</v>
+      </c>
       <c r="H21" s="14">
+        <v>4</v>
+      </c>
+      <c r="I21" s="14">
+        <v>4</v>
+      </c>
+      <c r="J21" s="14">
+        <v>4</v>
+      </c>
+      <c r="K21" s="14">
+        <v>4</v>
+      </c>
+      <c r="L21" s="14">
+        <v>4</v>
+      </c>
+      <c r="M21" s="14">
+        <v>4</v>
+      </c>
+      <c r="N21" s="14">
+        <v>4</v>
+      </c>
+      <c r="O21" s="14">
+        <v>4</v>
+      </c>
+      <c r="P21" s="14">
+        <v>4</v>
+      </c>
+      <c r="Q21" s="14">
+        <v>4</v>
+      </c>
+      <c r="R21" s="14">
+        <v>4</v>
+      </c>
+      <c r="S21" s="14">
+        <v>4</v>
+      </c>
+      <c r="T21" s="14">
         <v>4</v>
       </c>
       <c r="V21" s="15" t="e">
@@ -5513,7 +7880,49 @@
       <c r="E22" s="14">
         <v>3</v>
       </c>
+      <c r="F22" s="14">
+        <v>3</v>
+      </c>
+      <c r="G22" s="14">
+        <v>3</v>
+      </c>
       <c r="H22" s="14">
+        <v>3</v>
+      </c>
+      <c r="I22" s="14">
+        <v>3</v>
+      </c>
+      <c r="J22" s="14">
+        <v>3</v>
+      </c>
+      <c r="K22" s="14">
+        <v>3</v>
+      </c>
+      <c r="L22" s="14">
+        <v>3</v>
+      </c>
+      <c r="M22" s="14">
+        <v>3</v>
+      </c>
+      <c r="N22" s="14">
+        <v>3</v>
+      </c>
+      <c r="O22" s="14">
+        <v>3</v>
+      </c>
+      <c r="P22" s="14">
+        <v>3</v>
+      </c>
+      <c r="Q22" s="14">
+        <v>3</v>
+      </c>
+      <c r="R22" s="14">
+        <v>3</v>
+      </c>
+      <c r="S22" s="14">
+        <v>3</v>
+      </c>
+      <c r="T22" s="14">
         <v>3</v>
       </c>
       <c r="V22" s="15" t="e">
@@ -5529,11 +7938,11 @@
       </c>
     </row>
     <row r="23" spans="2:24" customFormat="false" ht="15.75">
-      <c r="B23" s="49" t="s">
+      <c r="B23" s="54" t="s">
         <v>107</v>
       </c>
-      <c r="C23" s="50"/>
-      <c r="D23" s="51"/>
+      <c r="C23" s="55"/>
+      <c r="D23" s="56"/>
       <c r="E23" s="18">
         <f t="shared" ref="E23:U23" si="2">SUM(E3:E22)</f>
         <v>0</v>
@@ -5622,66 +8031,66 @@
       <c r="B26" s="37" t="s">
         <v>108</v>
       </c>
-      <c r="C26" s="52" t="s">
+      <c r="C26" s="57" t="s">
         <v>109</v>
       </c>
-      <c r="D26" s="52"/>
+      <c r="D26" s="57"/>
       <c r="V26" s="3"/>
     </row>
     <row r="27" spans="2:22" customFormat="false" ht="31.5" customHeight="1">
       <c r="B27" s="38">
         <v>5</v>
       </c>
-      <c r="C27" s="47" t="s">
+      <c r="C27" s="52" t="s">
         <v>110</v>
       </c>
-      <c r="D27" s="48"/>
+      <c r="D27" s="53"/>
       <c r="V27" s="3"/>
     </row>
     <row r="28" spans="2:4" customFormat="false" ht="31.5" customHeight="1">
       <c r="B28" s="38">
         <v>4</v>
       </c>
-      <c r="C28" s="47" t="s">
+      <c r="C28" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="D28" s="48"/>
+      <c r="D28" s="53"/>
     </row>
     <row r="29" spans="2:4" customFormat="false" ht="31.5" customHeight="1">
       <c r="B29" s="38">
         <v>3</v>
       </c>
-      <c r="C29" s="47" t="s">
+      <c r="C29" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="D29" s="48"/>
+      <c r="D29" s="53"/>
     </row>
     <row r="30" spans="2:4" customFormat="false" ht="31.5" customHeight="1">
       <c r="B30" s="38">
         <v>2</v>
       </c>
-      <c r="C30" s="47" t="s">
+      <c r="C30" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="D30" s="48"/>
+      <c r="D30" s="53"/>
     </row>
     <row r="31" spans="2:4" customFormat="false" ht="31.5" customHeight="1">
       <c r="B31" s="38">
         <v>1</v>
       </c>
-      <c r="C31" s="47" t="s">
+      <c r="C31" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="D31" s="48"/>
+      <c r="D31" s="53"/>
     </row>
     <row r="32" spans="2:4" customFormat="false" ht="31.5" customHeight="1">
       <c r="B32" s="38">
         <v>0</v>
       </c>
-      <c r="C32" s="47" t="s">
+      <c r="C32" s="52" t="s">
         <v>115</v>
       </c>
-      <c r="D32" s="48"/>
+      <c r="D32" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
fix error caused by merge conflict
</commit_message>
<xml_diff>
--- a/app/views/employees/review/TranKhanhThuan-review.xlsx
+++ b/app/views/employees/review/TranKhanhThuan-review.xlsx
@@ -1919,11 +1919,8 @@
     <xf numFmtId="0" fontId="14" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1931,14 +1928,17 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -4386,10 +4386,10 @@
       <c r="B3" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="46"/>
+      <c r="D3" s="51"/>
       <c r="E3" s="3">
         <v>4</v>
       </c>
@@ -4458,10 +4458,10 @@
       <c r="B4" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="46"/>
+      <c r="D4" s="51"/>
       <c r="E4" s="3">
         <v>3</v>
       </c>
@@ -4530,10 +4530,10 @@
       <c r="B5" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="46"/>
+      <c r="D5" s="51"/>
       <c r="E5" s="3">
         <v>3</v>
       </c>
@@ -4602,10 +4602,10 @@
       <c r="B6" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="47" t="s">
+      <c r="C6" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="48"/>
+      <c r="D6" s="47"/>
       <c r="E6" s="3">
         <v>3</v>
       </c>
@@ -4674,10 +4674,10 @@
       <c r="B7" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="46"/>
+      <c r="D7" s="51"/>
       <c r="E7" s="3">
         <v>3</v>
       </c>
@@ -4746,10 +4746,10 @@
       <c r="B8" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="45" t="s">
+      <c r="C8" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="46"/>
+      <c r="D8" s="51"/>
       <c r="E8" s="3">
         <v>4</v>
       </c>
@@ -4818,10 +4818,10 @@
       <c r="B9" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="47" t="s">
+      <c r="C9" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="48"/>
+      <c r="D9" s="47"/>
       <c r="E9" s="3">
         <v>4</v>
       </c>
@@ -4890,10 +4890,10 @@
       <c r="B10" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="45" t="s">
+      <c r="C10" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="46"/>
+      <c r="D10" s="51"/>
       <c r="E10" s="3">
         <v>4</v>
       </c>
@@ -4962,10 +4962,10 @@
       <c r="B11" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="45" t="s">
+      <c r="C11" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="46"/>
+      <c r="D11" s="51"/>
       <c r="E11" s="3">
         <v>3</v>
       </c>
@@ -5034,10 +5034,10 @@
       <c r="B12" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="45" t="s">
+      <c r="C12" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="D12" s="46"/>
+      <c r="D12" s="51"/>
       <c r="E12" s="3">
         <v>3</v>
       </c>
@@ -5106,10 +5106,10 @@
       <c r="B13" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="45" t="s">
+      <c r="C13" s="50" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="46"/>
+      <c r="D13" s="51"/>
       <c r="E13" s="3">
         <v>4</v>
       </c>
@@ -5178,10 +5178,10 @@
       <c r="B14" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="45" t="s">
+      <c r="C14" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="46"/>
+      <c r="D14" s="51"/>
       <c r="E14" s="3">
         <v>3</v>
       </c>
@@ -5250,10 +5250,10 @@
       <c r="B15" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="45" t="s">
+      <c r="C15" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="D15" s="46"/>
+      <c r="D15" s="51"/>
       <c r="E15" s="3">
         <v>4</v>
       </c>
@@ -5322,10 +5322,10 @@
       <c r="B16" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="45" t="s">
+      <c r="C16" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="D16" s="46"/>
+      <c r="D16" s="51"/>
       <c r="E16" s="3">
         <v>4</v>
       </c>
@@ -5394,10 +5394,10 @@
       <c r="B17" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="45" t="s">
+      <c r="C17" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="D17" s="46"/>
+      <c r="D17" s="51"/>
       <c r="E17" s="3">
         <v>3</v>
       </c>
@@ -5466,10 +5466,10 @@
       <c r="B18" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="C18" s="45" t="s">
+      <c r="C18" s="50" t="s">
         <v>64</v>
       </c>
-      <c r="D18" s="46"/>
+      <c r="D18" s="51"/>
       <c r="E18" s="3">
         <v>4</v>
       </c>
@@ -5538,10 +5538,10 @@
       <c r="B19" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="C19" s="45" t="s">
+      <c r="C19" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="D19" s="46"/>
+      <c r="D19" s="51"/>
       <c r="E19" s="3">
         <v>3</v>
       </c>
@@ -5610,10 +5610,10 @@
       <c r="B20" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="45" t="s">
+      <c r="C20" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="D20" s="46"/>
+      <c r="D20" s="51"/>
       <c r="E20" s="3">
         <v>3</v>
       </c>
@@ -5682,10 +5682,10 @@
       <c r="B21" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="C21" s="45" t="s">
+      <c r="C21" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="D21" s="46"/>
+      <c r="D21" s="51"/>
       <c r="E21" s="3">
         <v>3</v>
       </c>
@@ -5754,10 +5754,10 @@
       <c r="B22" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="C22" s="45" t="s">
+      <c r="C22" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="D22" s="46"/>
+      <c r="D22" s="51"/>
       <c r="E22" s="3">
         <v>4</v>
       </c>
@@ -5826,10 +5826,10 @@
       <c r="B23" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="C23" s="45" t="s">
+      <c r="C23" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="D23" s="46"/>
+      <c r="D23" s="51"/>
       <c r="E23" s="3">
         <v>4</v>
       </c>
@@ -5898,10 +5898,10 @@
       <c r="B24" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="C24" s="47" t="s">
+      <c r="C24" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="D24" s="48"/>
+      <c r="D24" s="47"/>
       <c r="E24" s="3">
         <v>3</v>
       </c>
@@ -5969,10 +5969,10 @@
       <c r="B25" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="C25" s="47" t="s">
+      <c r="C25" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="D25" s="48"/>
+      <c r="D25" s="47"/>
       <c r="E25" s="3">
         <v>4</v>
       </c>
@@ -6040,10 +6040,10 @@
       <c r="B26" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="C26" s="45" t="s">
+      <c r="C26" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="D26" s="46"/>
+      <c r="D26" s="51"/>
       <c r="E26" s="3">
         <v>4</v>
       </c>
@@ -6111,10 +6111,10 @@
       <c r="B27" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="C27" s="47" t="s">
+      <c r="C27" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="D27" s="48"/>
+      <c r="D27" s="47"/>
       <c r="E27" s="3">
         <v>4</v>
       </c>
@@ -6259,83 +6259,86 @@
       <c r="B30" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="50" t="s">
+      <c r="C30" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="D30" s="50"/>
+      <c r="D30" s="48"/>
       <c r="E30" s="22"/>
     </row>
     <row r="31" spans="2:5" customFormat="false" ht="51.75" customHeight="1">
       <c r="B31" s="11">
         <v>5</v>
       </c>
-      <c r="C31" s="51" t="s">
+      <c r="C31" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="D31" s="51"/>
+      <c r="D31" s="49"/>
       <c r="E31" s="24"/>
     </row>
     <row r="32" spans="2:5" customFormat="false" ht="33.75" customHeight="1">
       <c r="B32" s="11">
         <v>4</v>
       </c>
-      <c r="C32" s="49" t="s">
+      <c r="C32" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="D32" s="49"/>
+      <c r="D32" s="45"/>
       <c r="E32" s="24"/>
     </row>
     <row r="33" spans="2:5" customFormat="false" ht="30" customHeight="1">
       <c r="B33" s="11">
         <v>3</v>
       </c>
-      <c r="C33" s="49" t="s">
+      <c r="C33" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="D33" s="49"/>
+      <c r="D33" s="45"/>
       <c r="E33" s="24"/>
     </row>
     <row r="34" spans="2:5" customFormat="false" ht="31.5" customHeight="1">
       <c r="B34" s="11">
         <v>2</v>
       </c>
-      <c r="C34" s="49" t="s">
+      <c r="C34" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="D34" s="49"/>
+      <c r="D34" s="45"/>
       <c r="E34" s="24"/>
     </row>
     <row r="35" spans="2:5" customFormat="false" ht="39" customHeight="1">
       <c r="B35" s="11">
         <v>1</v>
       </c>
-      <c r="C35" s="49" t="s">
+      <c r="C35" s="45" t="s">
         <v>81</v>
       </c>
-      <c r="D35" s="49"/>
+      <c r="D35" s="45"/>
       <c r="E35" s="24"/>
     </row>
     <row r="36" spans="2:5" customFormat="false" ht="36.75" customHeight="1">
       <c r="B36" s="11">
         <v>0</v>
       </c>
-      <c r="C36" s="49" t="s">
+      <c r="C36" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="D36" s="49"/>
+      <c r="D36" s="45"/>
       <c r="E36" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="C16:D16"/>
@@ -6348,18 +6351,15 @@
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
   </mergeCells>
   <pageMargins left="0.7086614173228347" right="0.7086614173228347" top="0.7480314960629921" bottom="0.7480314960629921" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="78" orientation="portrait" r:id="rId1"/>
@@ -6374,10 +6374,10 @@
   <dimension ref="A1:Y32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="E13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Y3" sqref="Y3"/>
+      <selection pane="bottomRight" activeCell="Y4" sqref="Y4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6546,7 +6546,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="Y3" s="40" t="e">
-        <f>SUM(X24, '熱意- nhiet_tinh'!X28, '考え方- tu_duy'!W28)</f>
+        <f>SUM(X23, '熱意- nhiet_tinh'!X28, '考え方- tu_duy'!W28)</f>
         <v>#DIV/0!</v>
       </c>
     </row>

</xml_diff>